<commit_message>
updates to filling out climate report. TODOs added for more information needed
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/Better-Climate-Challenge-Emissions-Reporting.xlsx
+++ b/src/assets/csv_templates/Better-Climate-Challenge-Emissions-Reporting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/txr/dev/VERIFI/src/assets/csv_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0FB430-EF1E-C049-AE11-993A45FDF155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4FFA17-C803-434A-9854-1F48FE4C8E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="17640" xr2:uid="{9E0B5763-0FE8-425F-B782-C4A4D911BFA4}"/>
   </bookViews>
@@ -20,20 +20,15 @@
     <sheet name="Display" sheetId="24" r:id="rId5"/>
     <sheet name="Data Validation" sheetId="2" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Display!$O$30:$O$39</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Display!$O$31:$O$37</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Display!$P$47:$P$55</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Display!$P$30:$P$39</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Display!$Q$31:$Q$37</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Display!$O$30:$O$39</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Display!$O$31:$O$37</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Display!$P$30:$P$39</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Display!$P$47:$P$55</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Display!$Q$31:$Q$37</definedName>
-    <definedName name="LIST_MeasureType">[1]Lists!$D$3:$D$9</definedName>
-    <definedName name="LIST_PropertyType">[1]Lists!$B$3:$B$7</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Comments!$A$1:$K$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Emissions Reduction Initiatives'!$A$1:$K$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Facility Emissions'!$A$1:$H$12</definedName>
@@ -444,7 +439,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="119">
   <si>
     <t>Instructions</t>
   </si>
@@ -1067,12 +1062,6 @@
   <si>
     <t>Other Fuel (Gasoline, Diesel, Propane) (MMBtu)</t>
   </si>
-  <si>
-    <t>100% Wind renewable energy.  Our site in Belgium completed converting its energy supply to 100% renewable wind power and carbon-neutral natural gas in May 2021. This results in an estimated annual reduction of 270 metric tons of CO2e emissions.</t>
-  </si>
-  <si>
-    <t>Boiler conversion from coal to natural gas:  By the end of 2021, we successfully completed the conversion of coal-fired boilers to natural gas at our Washington Works, WV site.</t>
-  </si>
 </sst>
 </file>
 
@@ -2010,14 +1999,7 @@
     <cellStyle name="Normal 3" xfId="4" xr:uid="{E0111CA2-60F9-49F9-A8D7-2399BECF48A9}"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="5" tint="-0.24994659260841701"/>
@@ -2027,13 +2009,6 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3301,18 +3276,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3601,18 +3576,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6558,100 +6533,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instructions"/>
-      <sheetName val="Data Display (EXAMPLE)"/>
-      <sheetName val="Report (Original)"/>
-      <sheetName val="Lists"/>
-      <sheetName val="Report Building A"/>
-      <sheetName val="Report Building B"/>
-      <sheetName val="2021"/>
-      <sheetName val="2022"/>
-      <sheetName val="Back End"/>
-      <sheetName val="Emissions Factors and Constants"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Office</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>Energy Efficiency</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>Retail</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>On-Site Renewables</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Warehouse</v>
-          </cell>
-          <cell r="D5" t="str">
-            <v>Off-Site Renewables</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Manufacturing</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>Grid Interactivity</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Multifamily</v>
-          </cell>
-          <cell r="D7" t="str">
-            <v>REC</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8" t="str">
-            <v>Carbon Offset</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9" t="str">
-            <v>Other</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6">
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Building A</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="7">
-          <cell r="N7">
-            <v>1118200</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -6955,7 +6836,7 @@
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7172,58 +7053,19 @@
         <f>IF($D$10=0, "Select Base Year",$D$10)</f>
         <v>Select Base Year</v>
       </c>
-      <c r="E12" s="52" t="str">
-        <f t="shared" ref="E12:Q12" si="0">IF($D$12="Select Base Year","",D12+1)</f>
-        <v/>
-      </c>
-      <c r="F12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="H12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="J12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="K12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="L12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="M12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="O12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="P12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="Q12" s="52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
     </row>
     <row r="13" spans="1:20" ht="6" customHeight="1"/>
     <row r="14" spans="1:20" ht="17.5" customHeight="1">
@@ -7528,47 +7370,47 @@
         <v>0</v>
       </c>
       <c r="F28" s="82">
-        <f t="shared" ref="F28:P28" si="1">IFERROR(IF(L10="Market-Based GHG Goal",SUM(F21,F27),SUM(F21,F26)), "")</f>
+        <f t="shared" ref="F28:P28" si="0">IFERROR(IF(L10="Market-Based GHG Goal",SUM(F21,F27),SUM(F21,F26)), "")</f>
         <v>0</v>
       </c>
       <c r="G28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="M28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P28" s="82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q28" s="82">
@@ -7670,51 +7512,51 @@
         <v/>
       </c>
       <c r="F33" s="82" t="str">
-        <f t="shared" ref="F33:Q33" si="2">IF(F28&lt;&gt;0,($D$28-F28), "")</f>
+        <f t="shared" ref="F33:Q33" si="1">IF(F28&lt;&gt;0,($D$28-F28), "")</f>
         <v/>
       </c>
       <c r="G33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="N33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="O33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="P33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q33" s="82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -7732,51 +7574,51 @@
         <v/>
       </c>
       <c r="F34" s="83" t="str">
-        <f t="shared" ref="F34:Q34" si="3">IF(F28&lt;&gt;0,F33/$D$28, "")</f>
+        <f t="shared" ref="F34:Q34" si="2">IF(F28&lt;&gt;0,F33/$D$28, "")</f>
         <v/>
       </c>
       <c r="G34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="K34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="L34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="M34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="N34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="O34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="P34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="Q34" s="83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -7858,43 +7700,43 @@
         <v>0</v>
       </c>
       <c r="H38" s="71">
-        <f t="shared" ref="H38:Q38" si="4">IF(H40&lt;&gt;0, SUM(H39:H40), 0)</f>
+        <f t="shared" ref="H38:Q38" si="3">IF(H40&lt;&gt;0, SUM(H39:H40), 0)</f>
         <v>0</v>
       </c>
       <c r="I38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q38" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -8014,59 +7856,59 @@
       </c>
       <c r="C44" s="112"/>
       <c r="D44" s="84">
-        <f t="shared" ref="D44:H44" si="5">D40-SUM(D41:D43)</f>
+        <f t="shared" ref="D44:H44" si="4">D40-SUM(D41:D43)</f>
         <v>0</v>
       </c>
       <c r="E44" s="84">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="84">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G44" s="84">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="84">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I44" s="84">
+        <f t="shared" ref="I44:Q44" si="5">I40-SUM(I41:I43)</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="84">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F44" s="84">
+      <c r="K44" s="84">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G44" s="84">
+      <c r="L44" s="84">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H44" s="84">
+      <c r="M44" s="84">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I44" s="84">
-        <f t="shared" ref="I44:Q44" si="6">I40-SUM(I41:I43)</f>
+      <c r="N44" s="84">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J44" s="84">
-        <f t="shared" si="6"/>
+      <c r="O44" s="84">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K44" s="84">
-        <f t="shared" si="6"/>
+      <c r="P44" s="84">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L44" s="84">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="84">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="N44" s="84">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O44" s="84">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P44" s="84">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
       <c r="Q44" s="84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S44" s="44"/>
@@ -8500,59 +8342,59 @@
       </c>
       <c r="C65" s="108"/>
       <c r="D65" s="82" t="str">
-        <f t="shared" ref="D65:Q65" si="7">IFERROR(IF(SUM(D38,D45:D64)&lt;&gt;0, SUM(D45:D64)+(D38*3.412), ""),"")</f>
+        <f t="shared" ref="D65:Q65" si="6">IFERROR(IF(SUM(D38,D45:D64)&lt;&gt;0, SUM(D45:D64)+(D38*3.412), ""),"")</f>
         <v/>
       </c>
       <c r="E65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="F65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="H65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="J65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="K65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="L65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="M65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="N65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="O65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Q65" s="82" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -8812,55 +8654,55 @@
       </c>
       <c r="C78" s="109"/>
       <c r="D78" s="82" t="str">
-        <f t="shared" ref="D78:P78" si="8">IFERROR(IF(SUM(D69:D77)&lt;&gt;0, SUM(D70:D77)+(D69*3.412), ""),"")</f>
+        <f t="shared" ref="D78:P78" si="7">IFERROR(IF(SUM(D69:D77)&lt;&gt;0, SUM(D70:D77)+(D69*3.412), ""),"")</f>
         <v/>
       </c>
       <c r="E78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="J78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="N78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="O78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="P78" s="82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="Q78" s="82" t="str">
@@ -8934,55 +8776,55 @@
         <v/>
       </c>
       <c r="E82" s="85">
-        <f t="shared" ref="E82:Q82" si="9">$D$28*(1-$D$9)</f>
+        <f t="shared" ref="E82:Q82" si="8">$D$28*(1-$D$9)</f>
         <v>0</v>
       </c>
       <c r="F82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="H82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="J82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="K82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="M82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="N82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="Q82" s="85">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -8995,55 +8837,55 @@
         <v>0</v>
       </c>
       <c r="E83" s="86" t="str">
-        <f t="shared" ref="E83:Q83" si="10">IF(E34&lt;&gt;"",E34-D34,"")</f>
+        <f t="shared" ref="E83:Q83" si="9">IF(E34&lt;&gt;"",E34-D34,"")</f>
         <v/>
       </c>
       <c r="F83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="L83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="N83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="P83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Q83" s="86" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -9053,59 +8895,59 @@
       </c>
       <c r="C84" s="54"/>
       <c r="D84" s="87" t="str">
-        <f t="shared" ref="D84:Q84" si="11">IF(D28&lt;&gt;0,SUM(D38*3.412,D45:D47),"")</f>
+        <f t="shared" ref="D84:Q84" si="10">IF(D28&lt;&gt;0,SUM(D38*3.412,D45:D47),"")</f>
         <v/>
       </c>
       <c r="E84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="G84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="J84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="M84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="N84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="O84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="P84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="Q84" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
@@ -9115,59 +8957,59 @@
       </c>
       <c r="C85" s="104"/>
       <c r="D85" s="88" t="str">
-        <f t="shared" ref="D85:Q85" si="12">IFERROR(D27/D84*1000, "")</f>
+        <f t="shared" ref="D85:Q85" si="11">IFERROR(D27/D84*1000, "")</f>
         <v/>
       </c>
       <c r="E85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="F85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="G85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="I85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="J85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="K85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="L85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="M85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="N85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="O85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="P85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="Q85" s="88" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -9177,59 +9019,59 @@
       </c>
       <c r="C86" s="104"/>
       <c r="D86" s="89" t="str">
-        <f t="shared" ref="D86:Q86" si="13">IFERROR(D26/D84*1000, "")</f>
+        <f t="shared" ref="D86:Q86" si="12">IFERROR(D26/D84*1000, "")</f>
         <v/>
       </c>
       <c r="E86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="F86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="H86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="J86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="M86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="N86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="O86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="P86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Q86" s="89" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
@@ -9239,59 +9081,59 @@
       </c>
       <c r="C87" s="54"/>
       <c r="D87" s="87" t="str">
-        <f t="shared" ref="D87:Q87" si="14">IF(D28&lt;&gt;0,$D84-D84,"")</f>
+        <f t="shared" ref="D87:Q87" si="13">IF(D28&lt;&gt;0,$D84-D84,"")</f>
         <v/>
       </c>
       <c r="E87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="F87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="G87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="H87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="J87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="L87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="M87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="N87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="O87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="P87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q87" s="87" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -9301,59 +9143,59 @@
       </c>
       <c r="C88" s="54"/>
       <c r="D88" s="87" t="str">
-        <f t="shared" ref="D88:Q88" si="15">IF(D28&lt;&gt;0,D39-$D39,"")</f>
+        <f t="shared" ref="D88:Q88" si="14">IF(D28&lt;&gt;0,D39-$D39,"")</f>
         <v/>
       </c>
       <c r="E88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="F88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="G88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="H88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="I88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="J88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="K88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="L88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="M88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="N88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="O88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="P88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="Q88" s="87" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -9363,59 +9205,59 @@
       </c>
       <c r="C89" s="54"/>
       <c r="D89" s="87" t="str">
-        <f t="shared" ref="D89:Q89" si="16">IF(D28&lt;&gt;0,SUM(D41:D43)-SUM($D41:$D43),"")</f>
+        <f t="shared" ref="D89:Q89" si="15">IF(D28&lt;&gt;0,SUM(D41:D43)-SUM($D41:$D43),"")</f>
         <v/>
       </c>
       <c r="E89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="F89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="I89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="J89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="K89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="L89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="N89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="O89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="P89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Q89" s="87" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -9425,59 +9267,59 @@
       </c>
       <c r="C90" s="54"/>
       <c r="D90" s="87" t="str">
-        <f t="shared" ref="D90:Q90" si="17">IF(D28&lt;&gt;0,D84*($D85-D85)/1000,"")</f>
+        <f t="shared" ref="D90:Q90" si="16">IF(D28&lt;&gt;0,D84*($D85-D85)/1000,"")</f>
         <v/>
       </c>
       <c r="E90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="F90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="G90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="H90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="I90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="J90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="K90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="L90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="M90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="N90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="O90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="P90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="Q90" s="87" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -9510,59 +9352,59 @@
       </c>
       <c r="C93" s="104"/>
       <c r="D93" s="87" t="str">
-        <f t="shared" ref="D93:Q93" si="18">IF(D28&lt;&gt;0,$D22-D22,"")</f>
+        <f t="shared" ref="D93:Q93" si="17">IF(D28&lt;&gt;0,$D22-D22,"")</f>
         <v/>
       </c>
       <c r="E93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="F93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="G93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="H93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="I93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="L93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="M93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="N93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="O93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="P93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="Q93" s="87" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
@@ -9572,59 +9414,59 @@
       </c>
       <c r="C94" s="104"/>
       <c r="D94" s="87" t="str">
-        <f t="shared" ref="D94:Q94" si="19">IF(D28&lt;&gt;0,$D23-D23,"")</f>
+        <f t="shared" ref="D94:Q94" si="18">IF(D28&lt;&gt;0,$D23-D23,"")</f>
         <v/>
       </c>
       <c r="E94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="F94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="G94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="H94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="I94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="J94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="K94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="L94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="N94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="O94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="P94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="Q94" s="87" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
@@ -9634,59 +9476,59 @@
       </c>
       <c r="C95" s="104"/>
       <c r="D95" s="87" t="str">
-        <f t="shared" ref="D95:Q95" si="20">IF(D28&lt;&gt;0,($D24+$D25)-(D24+D25),"")</f>
+        <f t="shared" ref="D95:Q95" si="19">IF(D28&lt;&gt;0,($D24+$D25)-(D24+D25),"")</f>
         <v/>
       </c>
       <c r="E95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="F95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="G95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="H95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="I95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="J95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="K95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="L95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="O95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="P95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="Q95" s="87" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
@@ -9696,59 +9538,59 @@
       </c>
       <c r="C96" s="104"/>
       <c r="D96" s="87" t="str">
-        <f t="shared" ref="D96:Q96" si="21">IF(D28&lt;&gt;0,D87*$D85/1000,"")</f>
+        <f t="shared" ref="D96:Q96" si="20">IF(D28&lt;&gt;0,D87*$D85/1000,"")</f>
         <v/>
       </c>
       <c r="E96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="F96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="G96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="H96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="J96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="K96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="L96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="M96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="N96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="O96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="P96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="Q96" s="87" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
@@ -9758,59 +9600,59 @@
       </c>
       <c r="C97" s="104"/>
       <c r="D97" s="87" t="str">
-        <f t="shared" ref="D97:Q97" si="22">IF(D28&lt;&gt;0,D88*$D86/1000,"")</f>
+        <f t="shared" ref="D97:Q97" si="21">IF(D28&lt;&gt;0,D88*$D86/1000,"")</f>
         <v/>
       </c>
       <c r="E97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="F97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="H97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="I97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="J97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="K97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="L97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="M97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="N97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="O97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="P97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="Q97" s="87" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
@@ -9820,59 +9662,59 @@
       </c>
       <c r="C98" s="104"/>
       <c r="D98" s="87" t="str">
-        <f t="shared" ref="D98:Q98" si="23">IF(D28&lt;&gt;0,D89*$D86/1000,"")</f>
+        <f t="shared" ref="D98:Q98" si="22">IF(D28&lt;&gt;0,D89*$D86/1000,"")</f>
         <v/>
       </c>
       <c r="E98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="F98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="G98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="H98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="I98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="J98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="K98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="L98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="M98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="O98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="Q98" s="87" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -9882,59 +9724,59 @@
       </c>
       <c r="C99" s="104"/>
       <c r="D99" s="87" t="str">
-        <f t="shared" ref="D99:Q99" si="24">IF(D28&lt;&gt;0,D90-D97-D98,"")</f>
+        <f t="shared" ref="D99:Q99" si="23">IF(D28&lt;&gt;0,D90-D97-D98,"")</f>
         <v/>
       </c>
       <c r="E99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="F99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="G99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="H99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="I99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="J99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="K99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="L99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="M99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="N99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="O99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="P99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="Q99" s="87" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v/>
       </c>
     </row>
@@ -9944,59 +9786,59 @@
       </c>
       <c r="C100" s="54"/>
       <c r="D100" s="90" t="str">
-        <f t="shared" ref="D100:Q100" si="25">IF(D28&lt;&gt;0,SUM(D93:D99),"")</f>
+        <f t="shared" ref="D100:Q100" si="24">IF(D28&lt;&gt;0,SUM(D93:D99),"")</f>
         <v/>
       </c>
       <c r="E100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="F100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="G100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="H100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="I100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="J100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="K100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="L100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="M100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="N100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="O100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="P100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="Q100" s="90" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -10132,7 +9974,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10263,12 +10105,8 @@
       <c r="S6" s="27"/>
     </row>
     <row r="7" spans="1:20" ht="57.75" customHeight="1">
-      <c r="B7" s="31">
-        <v>2021</v>
-      </c>
-      <c r="C7" s="136" t="s">
-        <v>119</v>
-      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="136"/>
       <c r="D7" s="132"/>
       <c r="E7" s="132"/>
       <c r="F7" s="132"/>
@@ -10288,12 +10126,8 @@
       <c r="T7" s="5"/>
     </row>
     <row r="8" spans="1:20" ht="63" customHeight="1">
-      <c r="B8" s="31">
-        <v>2021</v>
-      </c>
-      <c r="C8" s="132" t="s">
-        <v>120</v>
-      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="132"/>
       <c r="E8" s="132"/>
       <c r="F8" s="132"/>
@@ -10694,7 +10528,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11623,8 +11457,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:AC55"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -11698,57 +11532,57 @@
         <f>'Portfolio Emissions'!D12</f>
         <v>Select Base Year</v>
       </c>
-      <c r="Q11" s="52" t="str">
+      <c r="Q11" s="52">
         <f>'Portfolio Emissions'!E12</f>
-        <v/>
-      </c>
-      <c r="R11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="R11" s="52">
         <f>'Portfolio Emissions'!F12</f>
-        <v/>
-      </c>
-      <c r="S11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="S11" s="52">
         <f>'Portfolio Emissions'!G12</f>
-        <v/>
-      </c>
-      <c r="T11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="T11" s="52">
         <f>'Portfolio Emissions'!H12</f>
-        <v/>
-      </c>
-      <c r="U11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="U11" s="52">
         <f>'Portfolio Emissions'!I12</f>
-        <v/>
-      </c>
-      <c r="V11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="V11" s="52">
         <f>'Portfolio Emissions'!J12</f>
-        <v/>
-      </c>
-      <c r="W11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="W11" s="52">
         <f>'Portfolio Emissions'!K12</f>
-        <v/>
-      </c>
-      <c r="X11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="X11" s="52">
         <f>'Portfolio Emissions'!L12</f>
-        <v/>
-      </c>
-      <c r="Y11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="52">
         <f>'Portfolio Emissions'!M12</f>
-        <v/>
-      </c>
-      <c r="Z11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="52">
         <f>'Portfolio Emissions'!N12</f>
-        <v/>
-      </c>
-      <c r="AA11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="52">
         <f>'Portfolio Emissions'!O12</f>
-        <v/>
-      </c>
-      <c r="AB11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="52">
         <f>'Portfolio Emissions'!P12</f>
-        <v/>
-      </c>
-      <c r="AC11" s="52" t="str">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="52">
         <f>'Portfolio Emissions'!Q12</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:29" ht="16">
@@ -12264,10 +12098,10 @@
     <mergeCell ref="B3:P3"/>
   </mergeCells>
   <conditionalFormatting sqref="R30:R36">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>R30&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>R30&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add notes and facility performance to export report
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/Better-Climate-Challenge-Emissions-Reporting.xlsx
+++ b/src/assets/csv_templates/Better-Climate-Challenge-Emissions-Reporting.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/txr/dev/VERIFI/src/assets/csv_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4FFA17-C803-434A-9854-1F48FE4C8E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF9193D-B992-664E-8347-156C4E5B8D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="17640" xr2:uid="{9E0B5763-0FE8-425F-B782-C4A4D911BFA4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{9E0B5763-0FE8-425F-B782-C4A4D911BFA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio Emissions" sheetId="26" r:id="rId1"/>
     <sheet name="Emissions Reduction Initiatives" sheetId="17" r:id="rId2"/>
     <sheet name="Facility Emissions" sheetId="19" r:id="rId3"/>
     <sheet name="Comments" sheetId="21" r:id="rId4"/>
-    <sheet name="Display" sheetId="24" r:id="rId5"/>
-    <sheet name="Data Validation" sheetId="2" r:id="rId6"/>
+    <sheet name="Display" sheetId="24" state="hidden" r:id="rId5"/>
+    <sheet name="Data Validation" sheetId="2" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Display!$O$30:$O$39</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Display!$O$31:$O$37</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Display!$P$30:$P$39</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Display!$P$47:$P$55</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Display!$Q$31:$Q$37</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Display!$O$30:$O$39</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Display!$O$31:$O$37</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Display!$P$47:$P$55</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Display!$P$30:$P$39</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Display!$Q$31:$Q$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Comments!$A$1:$K$10</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Emissions Reduction Initiatives'!$A$1:$K$10</definedName>
@@ -3276,18 +3276,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3576,18 +3576,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -6835,7 +6835,7 @@
   </sheetPr>
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
@@ -10903,7 +10903,7 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
@@ -11457,7 +11457,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:AC55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update template with hardcoded value
</commit_message>
<xml_diff>
--- a/src/assets/csv_templates/Better-Climate-Challenge-Emissions-Reporting.xlsx
+++ b/src/assets/csv_templates/Better-Climate-Challenge-Emissions-Reporting.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83F21BF-220B-F74A-8F89-F18A44F21FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E61B2F-AC44-1243-90F5-728565D54C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25220" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio Emissions" sheetId="26" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Facility Emissions'!$A1:$H12</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Portfolio Emissions'!$A1:$I37</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1174,7 +1174,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="59">
     <font>
@@ -2085,13 +2085,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="37" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="39" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2100,7 +2100,7 @@
     <xf numFmtId="0" fontId="40" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="40" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="40" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2109,7 +2109,7 @@
     <xf numFmtId="0" fontId="41" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="41" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="41" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2118,13 +2118,13 @@
     <xf numFmtId="0" fontId="42" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="42" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="42" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2133,7 +2133,7 @@
     <xf numFmtId="0" fontId="42" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="42" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2142,7 +2142,7 @@
     <xf numFmtId="0" fontId="43" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="43" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="43" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2151,13 +2151,13 @@
     <xf numFmtId="0" fontId="44" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="44" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="44" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="42" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2252,90 +2252,11 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2367,6 +2288,15 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -2383,7 +2313,74 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2397,6 +2394,9 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2633,9 +2633,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2673,7 +2673,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2779,7 +2779,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2921,7 +2921,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2934,8 +2934,8 @@
   </sheetPr>
   <dimension ref="A1:AI632"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S143" sqref="S143"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A90" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S114" sqref="S114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15"/>
@@ -3071,24 +3071,24 @@
     </row>
     <row r="4" spans="1:35" ht="15" customHeight="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="154" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
-      <c r="H4" s="163"/>
-      <c r="I4" s="163"/>
-      <c r="J4" s="163"/>
-      <c r="K4" s="163"/>
-      <c r="L4" s="163"/>
-      <c r="M4" s="163"/>
-      <c r="N4" s="163"/>
-      <c r="O4" s="163"/>
-      <c r="P4" s="163"/>
-      <c r="Q4" s="178"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155"/>
+      <c r="H4" s="155"/>
+      <c r="I4" s="155"/>
+      <c r="J4" s="155"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="155"/>
+      <c r="M4" s="155"/>
+      <c r="N4" s="155"/>
+      <c r="O4" s="155"/>
+      <c r="P4" s="155"/>
+      <c r="Q4" s="156"/>
       <c r="R4" s="9"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -3110,24 +3110,24 @@
     </row>
     <row r="5" spans="1:35" ht="15" customHeight="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="177" t="s">
+      <c r="B5" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="163"/>
-      <c r="H5" s="163"/>
-      <c r="I5" s="163"/>
-      <c r="J5" s="163"/>
-      <c r="K5" s="163"/>
-      <c r="L5" s="163"/>
-      <c r="M5" s="163"/>
-      <c r="N5" s="163"/>
-      <c r="O5" s="163"/>
-      <c r="P5" s="163"/>
-      <c r="Q5" s="178"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
+      <c r="K5" s="155"/>
+      <c r="L5" s="155"/>
+      <c r="M5" s="155"/>
+      <c r="N5" s="155"/>
+      <c r="O5" s="155"/>
+      <c r="P5" s="155"/>
+      <c r="Q5" s="156"/>
       <c r="R5" s="10"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
@@ -3149,24 +3149,24 @@
     </row>
     <row r="6" spans="1:35" ht="15" customHeight="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="177" t="s">
+      <c r="B6" s="154" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="163"/>
-      <c r="K6" s="163"/>
-      <c r="L6" s="163"/>
-      <c r="M6" s="163"/>
-      <c r="N6" s="163"/>
-      <c r="O6" s="163"/>
-      <c r="P6" s="163"/>
-      <c r="Q6" s="178"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="155"/>
+      <c r="G6" s="155"/>
+      <c r="H6" s="155"/>
+      <c r="I6" s="155"/>
+      <c r="J6" s="155"/>
+      <c r="K6" s="155"/>
+      <c r="L6" s="155"/>
+      <c r="M6" s="155"/>
+      <c r="N6" s="155"/>
+      <c r="O6" s="155"/>
+      <c r="P6" s="155"/>
+      <c r="Q6" s="156"/>
       <c r="R6" s="10"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -3188,24 +3188,24 @@
     </row>
     <row r="7" spans="1:35" ht="15" customHeight="1">
       <c r="A7" s="6"/>
-      <c r="B7" s="177" t="s">
+      <c r="B7" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="163"/>
-      <c r="H7" s="163"/>
-      <c r="I7" s="163"/>
-      <c r="J7" s="163"/>
-      <c r="K7" s="163"/>
-      <c r="L7" s="163"/>
-      <c r="M7" s="163"/>
-      <c r="N7" s="163"/>
-      <c r="O7" s="163"/>
-      <c r="P7" s="163"/>
-      <c r="Q7" s="178"/>
+      <c r="C7" s="155"/>
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="155"/>
+      <c r="H7" s="155"/>
+      <c r="I7" s="155"/>
+      <c r="J7" s="155"/>
+      <c r="K7" s="155"/>
+      <c r="L7" s="155"/>
+      <c r="M7" s="155"/>
+      <c r="N7" s="155"/>
+      <c r="O7" s="155"/>
+      <c r="P7" s="155"/>
+      <c r="Q7" s="156"/>
       <c r="R7" s="10"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -3227,24 +3227,24 @@
     </row>
     <row r="8" spans="1:35" ht="15" customHeight="1">
       <c r="A8" s="6"/>
-      <c r="B8" s="179" t="s">
+      <c r="B8" s="157" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="180"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="180"/>
-      <c r="F8" s="180"/>
-      <c r="G8" s="180"/>
-      <c r="H8" s="180"/>
-      <c r="I8" s="180"/>
-      <c r="J8" s="180"/>
-      <c r="K8" s="180"/>
-      <c r="L8" s="180"/>
-      <c r="M8" s="180"/>
-      <c r="N8" s="180"/>
-      <c r="O8" s="180"/>
-      <c r="P8" s="180"/>
-      <c r="Q8" s="181"/>
+      <c r="C8" s="158"/>
+      <c r="D8" s="158"/>
+      <c r="E8" s="158"/>
+      <c r="F8" s="158"/>
+      <c r="G8" s="158"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="158"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="158"/>
+      <c r="L8" s="158"/>
+      <c r="M8" s="158"/>
+      <c r="N8" s="158"/>
+      <c r="O8" s="158"/>
+      <c r="P8" s="158"/>
+      <c r="Q8" s="159"/>
       <c r="R8" s="10"/>
       <c r="S8" s="6"/>
       <c r="T8" s="11"/>
@@ -3306,16 +3306,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="130"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="183"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="183"/>
-      <c r="J10" s="183"/>
-      <c r="K10" s="183"/>
-      <c r="L10" s="183"/>
-      <c r="M10" s="184"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="161"/>
+      <c r="F10" s="161"/>
+      <c r="G10" s="161"/>
+      <c r="H10" s="161"/>
+      <c r="I10" s="161"/>
+      <c r="J10" s="161"/>
+      <c r="K10" s="161"/>
+      <c r="L10" s="161"/>
+      <c r="M10" s="162"/>
       <c r="Q10" s="13"/>
       <c r="R10" s="14"/>
     </row>
@@ -3364,16 +3364,16 @@
       <c r="C12" s="133"/>
       <c r="D12" s="15"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="170" t="s">
+      <c r="F12" s="163" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="171"/>
-      <c r="H12" s="171"/>
-      <c r="I12" s="172"/>
-      <c r="J12" s="185"/>
-      <c r="K12" s="186"/>
-      <c r="L12" s="186"/>
-      <c r="M12" s="187"/>
+      <c r="G12" s="164"/>
+      <c r="H12" s="164"/>
+      <c r="I12" s="165"/>
+      <c r="J12" s="166"/>
+      <c r="K12" s="167"/>
+      <c r="L12" s="167"/>
+      <c r="M12" s="168"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
@@ -3405,16 +3405,16 @@
       <c r="C13" s="133"/>
       <c r="D13" s="16"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="170" t="s">
+      <c r="F13" s="163" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="171"/>
-      <c r="H13" s="171"/>
-      <c r="I13" s="172"/>
-      <c r="J13" s="188"/>
-      <c r="K13" s="174"/>
-      <c r="L13" s="174"/>
-      <c r="M13" s="175"/>
+      <c r="G13" s="164"/>
+      <c r="H13" s="164"/>
+      <c r="I13" s="165"/>
+      <c r="J13" s="169"/>
+      <c r="K13" s="170"/>
+      <c r="L13" s="170"/>
+      <c r="M13" s="171"/>
       <c r="N13" s="6"/>
       <c r="O13" s="17"/>
       <c r="P13" s="6"/>
@@ -3446,16 +3446,16 @@
       <c r="C14" s="132"/>
       <c r="D14" s="16"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="170" t="s">
+      <c r="F14" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="171"/>
-      <c r="H14" s="171"/>
-      <c r="I14" s="172"/>
-      <c r="J14" s="173"/>
-      <c r="K14" s="174"/>
-      <c r="L14" s="174"/>
-      <c r="M14" s="175"/>
+      <c r="G14" s="164"/>
+      <c r="H14" s="164"/>
+      <c r="I14" s="165"/>
+      <c r="J14" s="172"/>
+      <c r="K14" s="170"/>
+      <c r="L14" s="170"/>
+      <c r="M14" s="171"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
@@ -3597,24 +3597,24 @@
     </row>
     <row r="17" spans="1:35" ht="17.75" customHeight="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="173" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="165"/>
-      <c r="E17" s="165"/>
-      <c r="F17" s="165"/>
-      <c r="G17" s="165"/>
-      <c r="H17" s="165"/>
-      <c r="I17" s="165"/>
-      <c r="J17" s="165"/>
-      <c r="K17" s="165"/>
-      <c r="L17" s="165"/>
-      <c r="M17" s="165"/>
-      <c r="N17" s="165"/>
-      <c r="O17" s="165"/>
-      <c r="P17" s="165"/>
-      <c r="Q17" s="165"/>
+      <c r="C17" s="173"/>
+      <c r="D17" s="173"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
+      <c r="L17" s="173"/>
+      <c r="M17" s="173"/>
+      <c r="N17" s="173"/>
+      <c r="O17" s="173"/>
+      <c r="P17" s="173"/>
+      <c r="Q17" s="173"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
@@ -3673,10 +3673,10 @@
     </row>
     <row r="19" spans="1:35" s="19" customFormat="1" ht="22.25" customHeight="1">
       <c r="A19" s="20"/>
-      <c r="B19" s="176" t="s">
+      <c r="B19" s="174" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="176"/>
+      <c r="C19" s="174"/>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
@@ -3712,10 +3712,10 @@
     </row>
     <row r="20" spans="1:35" s="19" customFormat="1" ht="22.25" customHeight="1">
       <c r="A20" s="20"/>
-      <c r="B20" s="176" t="s">
+      <c r="B20" s="174" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="176"/>
+      <c r="C20" s="174"/>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
@@ -3788,24 +3788,24 @@
     </row>
     <row r="22" spans="1:35" ht="17.75" customHeight="1">
       <c r="A22" s="6"/>
-      <c r="B22" s="165" t="s">
+      <c r="B22" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="165"/>
-      <c r="D22" s="165"/>
-      <c r="E22" s="165"/>
-      <c r="F22" s="165"/>
-      <c r="G22" s="165"/>
-      <c r="H22" s="165"/>
-      <c r="I22" s="165"/>
-      <c r="J22" s="165"/>
-      <c r="K22" s="165"/>
-      <c r="L22" s="165"/>
-      <c r="M22" s="165"/>
-      <c r="N22" s="165"/>
-      <c r="O22" s="165"/>
-      <c r="P22" s="165"/>
-      <c r="Q22" s="165"/>
+      <c r="C22" s="173"/>
+      <c r="D22" s="173"/>
+      <c r="E22" s="173"/>
+      <c r="F22" s="173"/>
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173"/>
+      <c r="J22" s="173"/>
+      <c r="K22" s="173"/>
+      <c r="L22" s="173"/>
+      <c r="M22" s="173"/>
+      <c r="N22" s="173"/>
+      <c r="O22" s="173"/>
+      <c r="P22" s="173"/>
+      <c r="Q22" s="173"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
@@ -3864,10 +3864,10 @@
     </row>
     <row r="24" spans="1:35" ht="22.25" customHeight="1">
       <c r="A24" s="6"/>
-      <c r="B24" s="166" t="s">
+      <c r="B24" s="175" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="166"/>
+      <c r="C24" s="175"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
@@ -3884,8 +3884,8 @@
       <c r="Q24" s="25"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
-      <c r="T24" s="166"/>
-      <c r="U24" s="166"/>
+      <c r="T24" s="175"/>
+      <c r="U24" s="175"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
@@ -3903,10 +3903,10 @@
     </row>
     <row r="25" spans="1:35" ht="22.25" customHeight="1">
       <c r="A25" s="6"/>
-      <c r="B25" s="168" t="s">
+      <c r="B25" s="176" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="168"/>
+      <c r="C25" s="176"/>
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
@@ -3923,8 +3923,8 @@
       <c r="Q25" s="25"/>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
-      <c r="T25" s="169"/>
-      <c r="U25" s="169"/>
+      <c r="T25" s="177"/>
+      <c r="U25" s="177"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
@@ -3942,10 +3942,10 @@
     </row>
     <row r="26" spans="1:35" ht="22.25" customHeight="1">
       <c r="A26" s="6"/>
-      <c r="B26" s="168" t="s">
+      <c r="B26" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="168"/>
+      <c r="C26" s="176"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
@@ -3962,8 +3962,8 @@
       <c r="Q26" s="25"/>
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
-      <c r="T26" s="169"/>
-      <c r="U26" s="169"/>
+      <c r="T26" s="177"/>
+      <c r="U26" s="177"/>
       <c r="V26" s="6"/>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
@@ -3981,10 +3981,10 @@
     </row>
     <row r="27" spans="1:35" ht="22.25" customHeight="1">
       <c r="A27" s="6"/>
-      <c r="B27" s="168" t="s">
+      <c r="B27" s="176" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="168"/>
+      <c r="C27" s="176"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
@@ -4001,8 +4001,8 @@
       <c r="Q27" s="25"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
-      <c r="T27" s="169"/>
-      <c r="U27" s="169"/>
+      <c r="T27" s="177"/>
+      <c r="U27" s="177"/>
       <c r="V27" s="6"/>
       <c r="W27" s="6"/>
       <c r="X27" s="6"/>
@@ -4020,10 +4020,10 @@
     </row>
     <row r="28" spans="1:35" ht="22.25" customHeight="1">
       <c r="A28" s="6"/>
-      <c r="B28" s="168" t="s">
+      <c r="B28" s="176" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="168"/>
+      <c r="C28" s="176"/>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -4059,10 +4059,10 @@
     </row>
     <row r="29" spans="1:35" ht="22.25" customHeight="1">
       <c r="A29" s="6"/>
-      <c r="B29" s="166" t="s">
+      <c r="B29" s="175" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="166"/>
+      <c r="C29" s="175"/>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
@@ -4079,8 +4079,8 @@
       <c r="Q29" s="25"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
-      <c r="T29" s="166"/>
-      <c r="U29" s="166"/>
+      <c r="T29" s="175"/>
+      <c r="U29" s="175"/>
       <c r="V29" s="6"/>
       <c r="W29" s="6"/>
       <c r="X29" s="6"/>
@@ -4098,10 +4098,10 @@
     </row>
     <row r="30" spans="1:35" ht="22.25" customHeight="1">
       <c r="A30" s="6"/>
-      <c r="B30" s="166" t="s">
+      <c r="B30" s="175" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="166"/>
+      <c r="C30" s="175"/>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
@@ -4118,8 +4118,8 @@
       <c r="Q30" s="25"/>
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
-      <c r="T30" s="166"/>
-      <c r="U30" s="166"/>
+      <c r="T30" s="175"/>
+      <c r="U30" s="175"/>
       <c r="V30" s="6"/>
       <c r="W30" s="6"/>
       <c r="X30" s="6"/>
@@ -4137,10 +4137,10 @@
     </row>
     <row r="31" spans="1:35" ht="22.25" customHeight="1">
       <c r="A31" s="6"/>
-      <c r="B31" s="166" t="s">
+      <c r="B31" s="175" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="166"/>
+      <c r="C31" s="175"/>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
@@ -4176,10 +4176,10 @@
     </row>
     <row r="32" spans="1:35" ht="22.25" customHeight="1">
       <c r="A32" s="6"/>
-      <c r="B32" s="166" t="s">
+      <c r="B32" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="166"/>
+      <c r="C32" s="175"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
       <c r="F32" s="25"/>
@@ -4215,10 +4215,10 @@
     </row>
     <row r="33" spans="1:35" ht="22.25" customHeight="1">
       <c r="A33" s="6"/>
-      <c r="B33" s="166" t="s">
+      <c r="B33" s="175" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="166"/>
+      <c r="C33" s="175"/>
       <c r="D33" s="28">
         <f>IFERROR(IF($J$13="Market-Based GHG Goal",SUM(D24,D30,D32),SUM(D24,D29,D31)), "")</f>
         <v>0</v>
@@ -4277,8 +4277,8 @@
       </c>
       <c r="R33" s="6"/>
       <c r="S33" s="6"/>
-      <c r="T33" s="166"/>
-      <c r="U33" s="166"/>
+      <c r="T33" s="175"/>
+      <c r="U33" s="175"/>
       <c r="V33" s="6"/>
       <c r="W33" s="6"/>
       <c r="X33" s="6"/>
@@ -4296,10 +4296,10 @@
     </row>
     <row r="34" spans="1:35" ht="22.25" customHeight="1">
       <c r="A34" s="6"/>
-      <c r="B34" s="166" t="s">
+      <c r="B34" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="166"/>
+      <c r="C34" s="175"/>
       <c r="D34" s="25"/>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
@@ -4372,24 +4372,24 @@
     </row>
     <row r="36" spans="1:35" ht="17.75" customHeight="1">
       <c r="A36" s="6"/>
-      <c r="B36" s="165" t="s">
+      <c r="B36" s="173" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="165"/>
-      <c r="D36" s="165"/>
-      <c r="E36" s="165"/>
-      <c r="F36" s="165"/>
-      <c r="G36" s="165"/>
-      <c r="H36" s="165"/>
-      <c r="I36" s="165"/>
-      <c r="J36" s="165"/>
-      <c r="K36" s="165"/>
-      <c r="L36" s="165"/>
-      <c r="M36" s="165"/>
-      <c r="N36" s="165"/>
-      <c r="O36" s="165"/>
-      <c r="P36" s="165"/>
-      <c r="Q36" s="165"/>
+      <c r="C36" s="173"/>
+      <c r="D36" s="173"/>
+      <c r="E36" s="173"/>
+      <c r="F36" s="173"/>
+      <c r="G36" s="173"/>
+      <c r="H36" s="173"/>
+      <c r="I36" s="173"/>
+      <c r="J36" s="173"/>
+      <c r="K36" s="173"/>
+      <c r="L36" s="173"/>
+      <c r="M36" s="173"/>
+      <c r="N36" s="173"/>
+      <c r="O36" s="173"/>
+      <c r="P36" s="173"/>
+      <c r="Q36" s="173"/>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
       <c r="T36" s="6"/>
@@ -4448,10 +4448,10 @@
     </row>
     <row r="38" spans="1:35" ht="22.25" customHeight="1">
       <c r="A38" s="6"/>
-      <c r="B38" s="160" t="s">
+      <c r="B38" s="178" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="160"/>
+      <c r="C38" s="178"/>
       <c r="D38" s="28" t="str">
         <f>IF(D33&lt;&gt;0,($D$33-D33), "")</f>
         <v/>
@@ -4529,10 +4529,10 @@
     </row>
     <row r="39" spans="1:35" ht="22.25" customHeight="1">
       <c r="A39" s="6"/>
-      <c r="B39" s="160" t="s">
+      <c r="B39" s="178" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="160"/>
+      <c r="C39" s="178"/>
       <c r="D39" s="29" t="str">
         <f>IF(D33&lt;&gt;0,D38/$D$33, "")</f>
         <v/>
@@ -4647,24 +4647,24 @@
     </row>
     <row r="41" spans="1:35" ht="17.75" customHeight="1">
       <c r="A41" s="6"/>
-      <c r="B41" s="165" t="s">
+      <c r="B41" s="173" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="165"/>
-      <c r="D41" s="165"/>
-      <c r="E41" s="165"/>
-      <c r="F41" s="165"/>
-      <c r="G41" s="165"/>
-      <c r="H41" s="165"/>
-      <c r="I41" s="165"/>
-      <c r="J41" s="165"/>
-      <c r="K41" s="165"/>
-      <c r="L41" s="165"/>
-      <c r="M41" s="165"/>
-      <c r="N41" s="165"/>
-      <c r="O41" s="165"/>
-      <c r="P41" s="165"/>
-      <c r="Q41" s="165"/>
+      <c r="C41" s="173"/>
+      <c r="D41" s="173"/>
+      <c r="E41" s="173"/>
+      <c r="F41" s="173"/>
+      <c r="G41" s="173"/>
+      <c r="H41" s="173"/>
+      <c r="I41" s="173"/>
+      <c r="J41" s="173"/>
+      <c r="K41" s="173"/>
+      <c r="L41" s="173"/>
+      <c r="M41" s="173"/>
+      <c r="N41" s="173"/>
+      <c r="O41" s="173"/>
+      <c r="P41" s="173"/>
+      <c r="Q41" s="173"/>
       <c r="R41" s="6"/>
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
@@ -4723,10 +4723,10 @@
     </row>
     <row r="43" spans="1:35" s="30" customFormat="1" ht="22.25" customHeight="1">
       <c r="A43" s="31"/>
-      <c r="B43" s="160" t="s">
+      <c r="B43" s="178" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="160"/>
+      <c r="C43" s="178"/>
       <c r="D43" s="32">
         <f>IF(D45&lt;&gt;0, SUM(D44:D45), 0)</f>
         <v>0</v>
@@ -4804,10 +4804,10 @@
     </row>
     <row r="44" spans="1:35" ht="22.25" customHeight="1">
       <c r="A44" s="6"/>
-      <c r="B44" s="168" t="s">
+      <c r="B44" s="176" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="168"/>
+      <c r="C44" s="176"/>
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
@@ -4822,8 +4822,8 @@
       <c r="O44" s="33"/>
       <c r="P44" s="33"/>
       <c r="Q44" s="33"/>
-      <c r="S44" s="169"/>
-      <c r="T44" s="169"/>
+      <c r="S44" s="177"/>
+      <c r="T44" s="177"/>
       <c r="U44" s="6"/>
       <c r="V44" s="6"/>
       <c r="W44" s="6"/>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="45" spans="1:35" ht="22.25" customHeight="1">
       <c r="A45" s="6"/>
-      <c r="B45" s="168" t="s">
+      <c r="B45" s="176" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="168"/>
+      <c r="C45" s="176"/>
       <c r="D45" s="34"/>
       <c r="E45" s="34"/>
       <c r="F45" s="34"/>
@@ -4860,8 +4860,8 @@
       <c r="O45" s="35"/>
       <c r="P45" s="35"/>
       <c r="Q45" s="35"/>
-      <c r="S45" s="169"/>
-      <c r="T45" s="169"/>
+      <c r="S45" s="177"/>
+      <c r="T45" s="177"/>
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
       <c r="W45" s="6"/>
@@ -4880,10 +4880,10 @@
     </row>
     <row r="46" spans="1:35" ht="22.25" customHeight="1">
       <c r="A46" s="6"/>
-      <c r="B46" s="167" t="s">
+      <c r="B46" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="167"/>
+      <c r="C46" s="179"/>
       <c r="D46" s="34"/>
       <c r="E46" s="34"/>
       <c r="F46" s="34"/>
@@ -4918,10 +4918,10 @@
     </row>
     <row r="47" spans="1:35" ht="22.25" customHeight="1">
       <c r="A47" s="6"/>
-      <c r="B47" s="167" t="s">
+      <c r="B47" s="179" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="167"/>
+      <c r="C47" s="179"/>
       <c r="D47" s="34"/>
       <c r="E47" s="34"/>
       <c r="F47" s="34"/>
@@ -4956,10 +4956,10 @@
     </row>
     <row r="48" spans="1:35" ht="22.25" customHeight="1">
       <c r="A48" s="6"/>
-      <c r="B48" s="167" t="s">
+      <c r="B48" s="179" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="167"/>
+      <c r="C48" s="179"/>
       <c r="D48" s="36"/>
       <c r="E48" s="36"/>
       <c r="F48" s="36"/>
@@ -4974,8 +4974,8 @@
       <c r="O48" s="33"/>
       <c r="P48" s="33"/>
       <c r="Q48" s="33"/>
-      <c r="S48" s="169"/>
-      <c r="T48" s="169"/>
+      <c r="S48" s="177"/>
+      <c r="T48" s="177"/>
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
       <c r="W48" s="6"/>
@@ -4994,10 +4994,10 @@
     </row>
     <row r="49" spans="1:35" ht="22.25" customHeight="1">
       <c r="A49" s="6"/>
-      <c r="B49" s="167" t="s">
+      <c r="B49" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="167"/>
+      <c r="C49" s="179"/>
       <c r="D49" s="37">
         <f>D45-SUM(D46:D48)</f>
         <v>0</v>
@@ -5074,10 +5074,10 @@
     </row>
     <row r="50" spans="1:35" ht="22.25" customHeight="1">
       <c r="A50" s="6"/>
-      <c r="B50" s="160" t="s">
+      <c r="B50" s="178" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="160"/>
+      <c r="C50" s="178"/>
       <c r="D50" s="24"/>
       <c r="E50" s="24"/>
       <c r="F50" s="24"/>
@@ -5092,8 +5092,8 @@
       <c r="O50" s="33"/>
       <c r="P50" s="33"/>
       <c r="Q50" s="33"/>
-      <c r="S50" s="166"/>
-      <c r="T50" s="166"/>
+      <c r="S50" s="175"/>
+      <c r="T50" s="175"/>
       <c r="U50" s="6"/>
       <c r="V50" s="6"/>
       <c r="W50" s="6"/>
@@ -5112,10 +5112,10 @@
     </row>
     <row r="51" spans="1:35" ht="22.25" customHeight="1">
       <c r="A51" s="6"/>
-      <c r="B51" s="160" t="s">
+      <c r="B51" s="178" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="160"/>
+      <c r="C51" s="178"/>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
@@ -5150,10 +5150,10 @@
     </row>
     <row r="52" spans="1:35" ht="22.25" customHeight="1">
       <c r="A52" s="6"/>
-      <c r="B52" s="160" t="s">
+      <c r="B52" s="178" t="s">
         <v>44</v>
       </c>
-      <c r="C52" s="160"/>
+      <c r="C52" s="178"/>
       <c r="D52" s="24"/>
       <c r="E52" s="24"/>
       <c r="F52" s="24"/>
@@ -5188,10 +5188,10 @@
     </row>
     <row r="53" spans="1:35" ht="22.25" customHeight="1">
       <c r="A53" s="6"/>
-      <c r="B53" s="166" t="s">
+      <c r="B53" s="175" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="166"/>
+      <c r="C53" s="175"/>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
@@ -5206,8 +5206,8 @@
       <c r="O53" s="33"/>
       <c r="P53" s="33"/>
       <c r="Q53" s="33"/>
-      <c r="S53" s="162"/>
-      <c r="T53" s="162"/>
+      <c r="S53" s="180"/>
+      <c r="T53" s="180"/>
       <c r="U53" s="6"/>
       <c r="V53" s="6"/>
       <c r="W53" s="6"/>
@@ -5226,10 +5226,10 @@
     </row>
     <row r="54" spans="1:35" ht="22.25" customHeight="1">
       <c r="A54" s="6"/>
-      <c r="B54" s="163" t="s">
+      <c r="B54" s="155" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="163"/>
+      <c r="C54" s="155"/>
       <c r="D54" s="24"/>
       <c r="E54" s="24"/>
       <c r="F54" s="24"/>
@@ -5264,10 +5264,10 @@
     </row>
     <row r="55" spans="1:35" ht="22.25" customHeight="1">
       <c r="A55" s="6"/>
-      <c r="B55" s="163" t="s">
+      <c r="B55" s="155" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="163"/>
+      <c r="C55" s="155"/>
       <c r="D55" s="24"/>
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
@@ -5302,10 +5302,10 @@
     </row>
     <row r="56" spans="1:35" ht="22.25" customHeight="1">
       <c r="A56" s="6"/>
-      <c r="B56" s="163" t="s">
+      <c r="B56" s="155" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="163"/>
+      <c r="C56" s="155"/>
       <c r="D56" s="24"/>
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
@@ -5340,10 +5340,10 @@
     </row>
     <row r="57" spans="1:35" ht="22.25" customHeight="1">
       <c r="A57" s="6"/>
-      <c r="B57" s="163" t="s">
+      <c r="B57" s="155" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="163"/>
+      <c r="C57" s="155"/>
       <c r="D57" s="24"/>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
@@ -5378,10 +5378,10 @@
     </row>
     <row r="58" spans="1:35" ht="22.25" customHeight="1">
       <c r="A58" s="6"/>
-      <c r="B58" s="163" t="s">
+      <c r="B58" s="155" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="163"/>
+      <c r="C58" s="155"/>
       <c r="D58" s="24"/>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
@@ -5416,10 +5416,10 @@
     </row>
     <row r="59" spans="1:35" ht="22.25" customHeight="1">
       <c r="A59" s="6"/>
-      <c r="B59" s="161" t="s">
+      <c r="B59" s="181" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="161"/>
+      <c r="C59" s="181"/>
       <c r="D59" s="40"/>
       <c r="E59" s="40"/>
       <c r="F59" s="40"/>
@@ -5454,10 +5454,10 @@
     </row>
     <row r="60" spans="1:35" ht="22.25" customHeight="1">
       <c r="A60" s="6"/>
-      <c r="B60" s="161" t="s">
+      <c r="B60" s="181" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="161"/>
+      <c r="C60" s="181"/>
       <c r="D60" s="40"/>
       <c r="E60" s="40"/>
       <c r="F60" s="40"/>
@@ -5492,10 +5492,10 @@
     </row>
     <row r="61" spans="1:35" ht="22.25" customHeight="1">
       <c r="A61" s="6"/>
-      <c r="B61" s="161" t="s">
+      <c r="B61" s="181" t="s">
         <v>53</v>
       </c>
-      <c r="C61" s="161"/>
+      <c r="C61" s="181"/>
       <c r="D61" s="40"/>
       <c r="E61" s="40"/>
       <c r="F61" s="40"/>
@@ -5530,10 +5530,10 @@
     </row>
     <row r="62" spans="1:35" ht="22.25" customHeight="1">
       <c r="A62" s="6"/>
-      <c r="B62" s="161" t="s">
+      <c r="B62" s="181" t="s">
         <v>54</v>
       </c>
-      <c r="C62" s="161"/>
+      <c r="C62" s="181"/>
       <c r="D62" s="40"/>
       <c r="E62" s="40"/>
       <c r="F62" s="40"/>
@@ -5568,10 +5568,10 @@
     </row>
     <row r="63" spans="1:35" ht="22.25" customHeight="1">
       <c r="A63" s="6"/>
-      <c r="B63" s="161" t="s">
+      <c r="B63" s="181" t="s">
         <v>55</v>
       </c>
-      <c r="C63" s="161"/>
+      <c r="C63" s="181"/>
       <c r="D63" s="40"/>
       <c r="E63" s="40"/>
       <c r="F63" s="40"/>
@@ -5606,10 +5606,10 @@
     </row>
     <row r="64" spans="1:35" ht="22.25" customHeight="1">
       <c r="A64" s="6"/>
-      <c r="B64" s="161" t="s">
+      <c r="B64" s="181" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="161"/>
+      <c r="C64" s="181"/>
       <c r="D64" s="40"/>
       <c r="E64" s="40"/>
       <c r="F64" s="40"/>
@@ -5682,10 +5682,10 @@
     </row>
     <row r="66" spans="1:35" ht="22.25" customHeight="1">
       <c r="A66" s="6"/>
-      <c r="B66" s="161" t="s">
+      <c r="B66" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="C66" s="161"/>
+      <c r="C66" s="181"/>
       <c r="D66" s="40"/>
       <c r="E66" s="40"/>
       <c r="F66" s="40"/>
@@ -5758,10 +5758,10 @@
     </row>
     <row r="68" spans="1:35" ht="22.25" customHeight="1">
       <c r="A68" s="6"/>
-      <c r="B68" s="163" t="s">
+      <c r="B68" s="155" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="163"/>
+      <c r="C68" s="155"/>
       <c r="D68" s="24"/>
       <c r="E68" s="24"/>
       <c r="F68" s="24"/>
@@ -5796,10 +5796,10 @@
     </row>
     <row r="69" spans="1:35" ht="22.25" customHeight="1">
       <c r="A69" s="6"/>
-      <c r="B69" s="163" t="s">
+      <c r="B69" s="155" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="163"/>
+      <c r="C69" s="155"/>
       <c r="D69" s="24"/>
       <c r="E69" s="24"/>
       <c r="F69" s="24"/>
@@ -5834,10 +5834,10 @@
     </row>
     <row r="70" spans="1:35" ht="22.25" customHeight="1">
       <c r="A70" s="6"/>
-      <c r="B70" s="163" t="s">
+      <c r="B70" s="155" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="163"/>
+      <c r="C70" s="155"/>
       <c r="D70" s="28" t="str">
         <f>IFERROR(IF(SUM(D43,D50:D69)&lt;&gt;0, SUM(D50:D69)+(D43*3.412), ""), "")</f>
         <v/>
@@ -5952,24 +5952,24 @@
     </row>
     <row r="72" spans="1:35" ht="17.75" customHeight="1">
       <c r="A72" s="6"/>
-      <c r="B72" s="165" t="s">
+      <c r="B72" s="173" t="s">
         <v>63</v>
       </c>
-      <c r="C72" s="165"/>
-      <c r="D72" s="165"/>
-      <c r="E72" s="165"/>
-      <c r="F72" s="165"/>
-      <c r="G72" s="165"/>
-      <c r="H72" s="165"/>
-      <c r="I72" s="165"/>
-      <c r="J72" s="165"/>
-      <c r="K72" s="165"/>
-      <c r="L72" s="165"/>
-      <c r="M72" s="165"/>
-      <c r="N72" s="165"/>
-      <c r="O72" s="165"/>
-      <c r="P72" s="165"/>
-      <c r="Q72" s="165"/>
+      <c r="C72" s="173"/>
+      <c r="D72" s="173"/>
+      <c r="E72" s="173"/>
+      <c r="F72" s="173"/>
+      <c r="G72" s="173"/>
+      <c r="H72" s="173"/>
+      <c r="I72" s="173"/>
+      <c r="J72" s="173"/>
+      <c r="K72" s="173"/>
+      <c r="L72" s="173"/>
+      <c r="M72" s="173"/>
+      <c r="N72" s="173"/>
+      <c r="O72" s="173"/>
+      <c r="P72" s="173"/>
+      <c r="Q72" s="173"/>
       <c r="R72" s="6"/>
       <c r="S72" s="6"/>
       <c r="T72" s="6"/>
@@ -6028,10 +6028,10 @@
     </row>
     <row r="74" spans="1:35" s="30" customFormat="1" ht="22.25" customHeight="1">
       <c r="A74" s="31"/>
-      <c r="B74" s="161" t="s">
+      <c r="B74" s="181" t="s">
         <v>64</v>
       </c>
-      <c r="C74" s="161"/>
+      <c r="C74" s="181"/>
       <c r="D74" s="25"/>
       <c r="E74" s="25"/>
       <c r="F74" s="25"/>
@@ -6067,10 +6067,10 @@
     </row>
     <row r="75" spans="1:35" ht="22.25" customHeight="1">
       <c r="A75" s="6"/>
-      <c r="B75" s="161" t="s">
+      <c r="B75" s="181" t="s">
         <v>54</v>
       </c>
-      <c r="C75" s="161"/>
+      <c r="C75" s="181"/>
       <c r="D75" s="34"/>
       <c r="E75" s="34"/>
       <c r="F75" s="34"/>
@@ -6086,8 +6086,8 @@
       <c r="P75" s="33"/>
       <c r="Q75" s="33"/>
       <c r="R75" s="6"/>
-      <c r="S75" s="166"/>
-      <c r="T75" s="166"/>
+      <c r="S75" s="175"/>
+      <c r="T75" s="175"/>
       <c r="U75" s="6"/>
       <c r="V75" s="6"/>
       <c r="W75" s="6"/>
@@ -6106,10 +6106,10 @@
     </row>
     <row r="76" spans="1:35" ht="22.25" customHeight="1">
       <c r="A76" s="6"/>
-      <c r="B76" s="161" t="s">
+      <c r="B76" s="181" t="s">
         <v>55</v>
       </c>
-      <c r="C76" s="161"/>
+      <c r="C76" s="181"/>
       <c r="D76" s="25"/>
       <c r="E76" s="25"/>
       <c r="F76" s="25"/>
@@ -6145,10 +6145,10 @@
     </row>
     <row r="77" spans="1:35" ht="22.25" customHeight="1">
       <c r="A77" s="6"/>
-      <c r="B77" s="161" t="s">
+      <c r="B77" s="181" t="s">
         <v>56</v>
       </c>
-      <c r="C77" s="161"/>
+      <c r="C77" s="181"/>
       <c r="D77" s="25"/>
       <c r="E77" s="25"/>
       <c r="F77" s="25"/>
@@ -6164,8 +6164,8 @@
       <c r="P77" s="33"/>
       <c r="Q77" s="33"/>
       <c r="R77" s="6"/>
-      <c r="S77" s="162"/>
-      <c r="T77" s="162"/>
+      <c r="S77" s="180"/>
+      <c r="T77" s="180"/>
       <c r="U77" s="6"/>
       <c r="V77" s="6"/>
       <c r="W77" s="6"/>
@@ -6223,10 +6223,10 @@
     </row>
     <row r="79" spans="1:35" ht="22.25" customHeight="1">
       <c r="A79" s="6"/>
-      <c r="B79" s="161" t="s">
+      <c r="B79" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="C79" s="161"/>
+      <c r="C79" s="181"/>
       <c r="D79" s="25"/>
       <c r="E79" s="25"/>
       <c r="F79" s="25"/>
@@ -6301,10 +6301,10 @@
     </row>
     <row r="81" spans="1:35" ht="22.25" customHeight="1">
       <c r="A81" s="6"/>
-      <c r="B81" s="163" t="s">
+      <c r="B81" s="155" t="s">
         <v>61</v>
       </c>
-      <c r="C81" s="163"/>
+      <c r="C81" s="155"/>
       <c r="D81" s="25"/>
       <c r="E81" s="25"/>
       <c r="F81" s="25"/>
@@ -6340,10 +6340,10 @@
     </row>
     <row r="82" spans="1:35" ht="22.25" customHeight="1">
       <c r="A82" s="6"/>
-      <c r="B82" s="163" t="s">
+      <c r="B82" s="155" t="s">
         <v>61</v>
       </c>
-      <c r="C82" s="163"/>
+      <c r="C82" s="155"/>
       <c r="D82" s="25"/>
       <c r="E82" s="25"/>
       <c r="F82" s="25"/>
@@ -6378,10 +6378,10 @@
       <c r="AI82" s="6"/>
     </row>
     <row r="83" spans="1:35" ht="22.25" customHeight="1">
-      <c r="B83" s="164" t="s">
+      <c r="B83" s="182" t="s">
         <v>65</v>
       </c>
-      <c r="C83" s="164"/>
+      <c r="C83" s="182"/>
       <c r="D83" s="135" t="str">
         <f>IFERROR(IF(SUM(D74:D82)&lt;&gt;0, SUM(D75:D82)+(D74*3.412), ""),"")</f>
         <v/>
@@ -6478,24 +6478,24 @@
     </row>
     <row r="85" spans="1:35" ht="17.75" customHeight="1">
       <c r="A85" s="6"/>
-      <c r="B85" s="165" t="s">
+      <c r="B85" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="C85" s="165"/>
-      <c r="D85" s="165"/>
-      <c r="E85" s="165"/>
-      <c r="F85" s="165"/>
-      <c r="G85" s="165"/>
-      <c r="H85" s="165"/>
-      <c r="I85" s="165"/>
-      <c r="J85" s="165"/>
-      <c r="K85" s="165"/>
-      <c r="L85" s="165"/>
-      <c r="M85" s="165"/>
-      <c r="N85" s="165"/>
-      <c r="O85" s="165"/>
-      <c r="P85" s="165"/>
-      <c r="Q85" s="165"/>
+      <c r="C85" s="173"/>
+      <c r="D85" s="173"/>
+      <c r="E85" s="173"/>
+      <c r="F85" s="173"/>
+      <c r="G85" s="173"/>
+      <c r="H85" s="173"/>
+      <c r="I85" s="173"/>
+      <c r="J85" s="173"/>
+      <c r="K85" s="173"/>
+      <c r="L85" s="173"/>
+      <c r="M85" s="173"/>
+      <c r="N85" s="173"/>
+      <c r="O85" s="173"/>
+      <c r="P85" s="173"/>
+      <c r="Q85" s="173"/>
       <c r="R85" s="6"/>
       <c r="S85" s="6"/>
       <c r="T85" s="6"/>
@@ -6554,10 +6554,10 @@
     </row>
     <row r="87" spans="1:35" s="22" customFormat="1" ht="22.25" customHeight="1">
       <c r="A87" s="11"/>
-      <c r="B87" s="160" t="s">
+      <c r="B87" s="178" t="s">
         <v>67</v>
       </c>
-      <c r="C87" s="160"/>
+      <c r="C87" s="178"/>
       <c r="D87" s="136" t="str">
         <f>IFERROR(IF(D70&lt;&gt;0,SUMPRODUCT(D$44:D$69,'Data Validation'!$I$26:$I$51)*1000/D$19, ""),"")</f>
         <v/>
@@ -6635,10 +6635,10 @@
     </row>
     <row r="88" spans="1:35" s="22" customFormat="1" ht="22.25" customHeight="1">
       <c r="A88" s="11"/>
-      <c r="B88" s="160" t="s">
+      <c r="B88" s="178" t="s">
         <v>68</v>
       </c>
-      <c r="C88" s="160"/>
+      <c r="C88" s="178"/>
       <c r="D88" s="137" t="str">
         <f>IFERROR(IF(D70&lt;&gt;0,($D$87-D87)/D87,""),"")</f>
         <v/>
@@ -6716,10 +6716,10 @@
     </row>
     <row r="89" spans="1:35" s="30" customFormat="1" ht="22.25" customHeight="1">
       <c r="A89" s="31"/>
-      <c r="B89" s="160" t="s">
+      <c r="B89" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="C89" s="160"/>
+      <c r="C89" s="178"/>
       <c r="D89" s="136" t="str">
         <f>IFERROR(IF(D70&lt;&gt;0,SUMPRODUCT(D$44:D$69,'Data Validation'!$H$26:$H$51,'Data Validation'!$I$26:$I$51)*1000/D$19, ""),"")</f>
         <v/>
@@ -6797,10 +6797,10 @@
     </row>
     <row r="90" spans="1:35" s="30" customFormat="1" ht="22.25" customHeight="1">
       <c r="A90" s="31"/>
-      <c r="B90" s="160" t="s">
+      <c r="B90" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="C90" s="160"/>
+      <c r="C90" s="178"/>
       <c r="D90" s="137" t="str">
         <f t="shared" ref="D90:Q90" si="9">IFERROR(IF(D70&lt;&gt;0,($D$89-D89)/D89,""),"")</f>
         <v/>
@@ -6878,10 +6878,10 @@
     </row>
     <row r="91" spans="1:35" s="30" customFormat="1" ht="22.25" customHeight="1">
       <c r="A91" s="31"/>
-      <c r="B91" s="160" t="s">
+      <c r="B91" s="178" t="s">
         <v>71</v>
       </c>
-      <c r="C91" s="160"/>
+      <c r="C91" s="178"/>
       <c r="D91" s="138"/>
       <c r="E91" s="138"/>
       <c r="F91" s="138"/>
@@ -6954,24 +6954,24 @@
     </row>
     <row r="93" spans="1:35" ht="17.75" customHeight="1">
       <c r="A93" s="44"/>
-      <c r="B93" s="159" t="s">
+      <c r="B93" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="C93" s="159"/>
-      <c r="D93" s="159"/>
-      <c r="E93" s="159"/>
-      <c r="F93" s="159"/>
-      <c r="G93" s="159"/>
-      <c r="H93" s="159"/>
-      <c r="I93" s="159"/>
-      <c r="J93" s="159"/>
-      <c r="K93" s="159"/>
-      <c r="L93" s="159"/>
-      <c r="M93" s="159"/>
-      <c r="N93" s="159"/>
-      <c r="O93" s="159"/>
-      <c r="P93" s="159"/>
-      <c r="Q93" s="159"/>
+      <c r="C93" s="183"/>
+      <c r="D93" s="183"/>
+      <c r="E93" s="183"/>
+      <c r="F93" s="183"/>
+      <c r="G93" s="183"/>
+      <c r="H93" s="183"/>
+      <c r="I93" s="183"/>
+      <c r="J93" s="183"/>
+      <c r="K93" s="183"/>
+      <c r="L93" s="183"/>
+      <c r="M93" s="183"/>
+      <c r="N93" s="183"/>
+      <c r="O93" s="183"/>
+      <c r="P93" s="183"/>
+      <c r="Q93" s="183"/>
       <c r="R93" s="44"/>
       <c r="S93" s="44"/>
       <c r="T93" s="44"/>
@@ -7030,10 +7030,10 @@
     </row>
     <row r="95" spans="1:35" s="48" customFormat="1" ht="22.25" customHeight="1">
       <c r="A95" s="49"/>
-      <c r="B95" s="156" t="s">
+      <c r="B95" s="184" t="s">
         <v>73</v>
       </c>
-      <c r="C95" s="156"/>
+      <c r="C95" s="184"/>
       <c r="D95" s="139" t="str">
         <f>IF(D33&lt;&gt;0,$D$33*(1-$D$12),"")</f>
         <v/>
@@ -7111,10 +7111,10 @@
     </row>
     <row r="96" spans="1:35" s="48" customFormat="1" ht="22.25" customHeight="1">
       <c r="A96" s="49"/>
-      <c r="B96" s="156" t="s">
+      <c r="B96" s="184" t="s">
         <v>74</v>
       </c>
-      <c r="C96" s="156"/>
+      <c r="C96" s="184"/>
       <c r="D96" s="140">
         <v>0</v>
       </c>
@@ -7272,10 +7272,10 @@
     </row>
     <row r="98" spans="1:35" ht="22.25" customHeight="1">
       <c r="A98" s="44"/>
-      <c r="B98" s="158" t="s">
+      <c r="B98" s="185" t="s">
         <v>76</v>
       </c>
-      <c r="C98" s="158"/>
+      <c r="C98" s="185"/>
       <c r="D98" s="141" t="str">
         <f t="shared" ref="D98:Q98" si="13">IFERROR(D30/D97*1000, "")</f>
         <v/>
@@ -7353,10 +7353,10 @@
     </row>
     <row r="99" spans="1:35" ht="27.75" customHeight="1">
       <c r="A99" s="44"/>
-      <c r="B99" s="158" t="s">
+      <c r="B99" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="C99" s="158"/>
+      <c r="C99" s="185"/>
       <c r="D99" s="142" t="str">
         <f t="shared" ref="D99:Q99" si="14">IFERROR(D29/D97*1000, "")</f>
         <v/>
@@ -7834,10 +7834,10 @@
     </row>
     <row r="106" spans="1:35" ht="34.25" customHeight="1">
       <c r="A106" s="44"/>
-      <c r="B106" s="158" t="s">
+      <c r="B106" s="185" t="s">
         <v>83</v>
       </c>
-      <c r="C106" s="158"/>
+      <c r="C106" s="185"/>
       <c r="D106" s="139" t="str">
         <f t="shared" ref="D106:Q106" si="19">IF(D33&lt;&gt;0,$D25-D25,"")</f>
         <v/>
@@ -7915,10 +7915,10 @@
     </row>
     <row r="107" spans="1:35" ht="34.25" customHeight="1">
       <c r="A107" s="44"/>
-      <c r="B107" s="158" t="s">
+      <c r="B107" s="185" t="s">
         <v>84</v>
       </c>
-      <c r="C107" s="158"/>
+      <c r="C107" s="185"/>
       <c r="D107" s="139" t="str">
         <f t="shared" ref="D107:Q107" si="20">IF(D33&lt;&gt;0,$D26-D26,"")</f>
         <v/>
@@ -7996,10 +7996,10 @@
     </row>
     <row r="108" spans="1:35" ht="34.25" customHeight="1">
       <c r="A108" s="44"/>
-      <c r="B108" s="158" t="s">
+      <c r="B108" s="185" t="s">
         <v>85</v>
       </c>
-      <c r="C108" s="158"/>
+      <c r="C108" s="185"/>
       <c r="D108" s="139" t="str">
         <f t="shared" ref="D108:Q108" si="21">IF(D33&lt;&gt;0,($D27+$D28)-(D27+D28),"")</f>
         <v/>
@@ -8077,10 +8077,10 @@
     </row>
     <row r="109" spans="1:35" ht="34.25" customHeight="1">
       <c r="A109" s="44"/>
-      <c r="B109" s="158" t="s">
+      <c r="B109" s="185" t="s">
         <v>86</v>
       </c>
-      <c r="C109" s="158"/>
+      <c r="C109" s="185"/>
       <c r="D109" s="139" t="str">
         <f>IF(D33&lt;&gt;0,IF($J$13="Market-Based GHG Goal",D100*$D98/1000,D100*$D99/1000),"")</f>
         <v/>
@@ -8158,10 +8158,10 @@
     </row>
     <row r="110" spans="1:35" ht="34.25" customHeight="1">
       <c r="A110" s="44"/>
-      <c r="B110" s="158" t="s">
+      <c r="B110" s="185" t="s">
         <v>87</v>
       </c>
-      <c r="C110" s="158"/>
+      <c r="C110" s="185"/>
       <c r="D110" s="139" t="str">
         <f t="shared" ref="D110:Q110" si="23">IF(D33&lt;&gt;0,D101*$D99/1000,"")</f>
         <v/>
@@ -8239,10 +8239,10 @@
     </row>
     <row r="111" spans="1:35" ht="34.25" customHeight="1">
       <c r="A111" s="44"/>
-      <c r="B111" s="158" t="s">
+      <c r="B111" s="185" t="s">
         <v>88</v>
       </c>
-      <c r="C111" s="158"/>
+      <c r="C111" s="185"/>
       <c r="D111" s="139" t="str">
         <f>IF(D33&lt;&gt;0,IF($J$13="Market-Based GHG Goal",D102*$D99/1000,0),"")</f>
         <v/>
@@ -8320,10 +8320,10 @@
     </row>
     <row r="112" spans="1:35" ht="34.25" customHeight="1">
       <c r="A112" s="44"/>
-      <c r="B112" s="158" t="s">
+      <c r="B112" s="185" t="s">
         <v>89</v>
       </c>
-      <c r="C112" s="158"/>
+      <c r="C112" s="185"/>
       <c r="D112" s="139" t="str">
         <f t="shared" ref="D112:Q112" si="25">IF(D33&lt;&gt;0,D103-D110-D111,"")</f>
         <v/>
@@ -8513,24 +8513,24 @@
     </row>
     <row r="115" spans="1:35" ht="18" customHeight="1">
       <c r="A115" s="44"/>
-      <c r="B115" s="159" t="s">
+      <c r="B115" s="183" t="s">
         <v>91</v>
       </c>
-      <c r="C115" s="159"/>
-      <c r="D115" s="159"/>
-      <c r="E115" s="159"/>
-      <c r="F115" s="159"/>
-      <c r="G115" s="159"/>
-      <c r="H115" s="159"/>
-      <c r="I115" s="159"/>
-      <c r="J115" s="159"/>
-      <c r="K115" s="159"/>
-      <c r="L115" s="159"/>
-      <c r="M115" s="159"/>
-      <c r="N115" s="159"/>
-      <c r="O115" s="159"/>
-      <c r="P115" s="159"/>
-      <c r="Q115" s="159"/>
+      <c r="C115" s="183"/>
+      <c r="D115" s="183"/>
+      <c r="E115" s="183"/>
+      <c r="F115" s="183"/>
+      <c r="G115" s="183"/>
+      <c r="H115" s="183"/>
+      <c r="I115" s="183"/>
+      <c r="J115" s="183"/>
+      <c r="K115" s="183"/>
+      <c r="L115" s="183"/>
+      <c r="M115" s="183"/>
+      <c r="N115" s="183"/>
+      <c r="O115" s="183"/>
+      <c r="P115" s="183"/>
+      <c r="Q115" s="183"/>
       <c r="R115" s="44"/>
       <c r="V115" s="44"/>
       <c r="W115" s="44"/>
@@ -8583,24 +8583,52 @@
     </row>
     <row r="117" spans="1:35" ht="22.25" customHeight="1">
       <c r="A117" s="44"/>
-      <c r="B117" s="156" t="s">
+      <c r="B117" s="184" t="s">
         <v>92</v>
       </c>
-      <c r="C117" s="156"/>
-      <c r="D117" s="144"/>
-      <c r="E117" s="144"/>
-      <c r="F117" s="144"/>
-      <c r="G117" s="144"/>
-      <c r="H117" s="144"/>
-      <c r="I117" s="144"/>
-      <c r="J117" s="144"/>
-      <c r="K117" s="144"/>
-      <c r="L117" s="144"/>
-      <c r="M117" s="144"/>
-      <c r="N117" s="144"/>
-      <c r="O117" s="144"/>
-      <c r="P117" s="144"/>
-      <c r="Q117" s="144"/>
+      <c r="C117" s="184"/>
+      <c r="D117" s="144">
+        <v>109</v>
+      </c>
+      <c r="E117" s="144">
+        <v>109</v>
+      </c>
+      <c r="F117" s="144">
+        <v>109</v>
+      </c>
+      <c r="G117" s="144">
+        <v>109</v>
+      </c>
+      <c r="H117" s="144">
+        <v>109</v>
+      </c>
+      <c r="I117" s="144">
+        <v>109</v>
+      </c>
+      <c r="J117" s="144">
+        <v>109</v>
+      </c>
+      <c r="K117" s="144">
+        <v>109</v>
+      </c>
+      <c r="L117" s="144">
+        <v>109</v>
+      </c>
+      <c r="M117" s="144">
+        <v>109</v>
+      </c>
+      <c r="N117" s="144">
+        <v>109</v>
+      </c>
+      <c r="O117" s="144">
+        <v>109</v>
+      </c>
+      <c r="P117" s="144">
+        <v>109</v>
+      </c>
+      <c r="Q117" s="144">
+        <v>109</v>
+      </c>
       <c r="R117" s="44"/>
       <c r="V117" s="44"/>
       <c r="W117" s="44"/>
@@ -8619,10 +8647,10 @@
     </row>
     <row r="118" spans="1:35" ht="22.5" customHeight="1">
       <c r="A118" s="44"/>
-      <c r="B118" s="156" t="s">
+      <c r="B118" s="184" t="s">
         <v>93</v>
       </c>
-      <c r="C118" s="156"/>
+      <c r="C118" s="184"/>
       <c r="D118" s="139">
         <f>D45*D117*3.412/1000</f>
         <v>0</v>
@@ -8697,10 +8725,10 @@
     </row>
     <row r="119" spans="1:35" ht="22.5" customHeight="1">
       <c r="A119" s="44"/>
-      <c r="B119" s="156" t="s">
+      <c r="B119" s="184" t="s">
         <v>94</v>
       </c>
-      <c r="C119" s="156"/>
+      <c r="C119" s="184"/>
       <c r="D119" s="139">
         <f>D49*D117*3.412/1000</f>
         <v>0</v>
@@ -8775,10 +8803,10 @@
     </row>
     <row r="120" spans="1:35" ht="22.5" customHeight="1">
       <c r="A120" s="44"/>
-      <c r="B120" s="156" t="s">
+      <c r="B120" s="184" t="s">
         <v>95</v>
       </c>
-      <c r="C120" s="156"/>
+      <c r="C120" s="184"/>
       <c r="D120" s="139">
         <f t="shared" ref="D120:Q120" si="29">D50*66.4/1000</f>
         <v>0</v>
@@ -8856,10 +8884,10 @@
     </row>
     <row r="121" spans="1:35" ht="22.5" customHeight="1">
       <c r="A121" s="44"/>
-      <c r="B121" s="156" t="s">
+      <c r="B121" s="184" t="s">
         <v>96</v>
       </c>
-      <c r="C121" s="156"/>
+      <c r="C121" s="184"/>
       <c r="D121" s="139">
         <f t="shared" ref="D121:Q121" si="30">D51*66.5/1000</f>
         <v>0</v>
@@ -8937,10 +8965,10 @@
     </row>
     <row r="122" spans="1:35" ht="22.5" customHeight="1">
       <c r="A122" s="44"/>
-      <c r="B122" s="156" t="s">
+      <c r="B122" s="184" t="s">
         <v>97</v>
       </c>
-      <c r="C122" s="156"/>
+      <c r="C122" s="184"/>
       <c r="D122" s="139">
         <f t="shared" ref="D122:Q122" si="31">D52*58.617/1000</f>
         <v>0</v>
@@ -9018,10 +9046,10 @@
     </row>
     <row r="123" spans="1:35" ht="22.5" customHeight="1">
       <c r="A123" s="44"/>
-      <c r="B123" s="157" t="s">
+      <c r="B123" s="188" t="s">
         <v>98</v>
       </c>
-      <c r="C123" s="157"/>
+      <c r="C123" s="188"/>
       <c r="D123" s="139">
         <f t="shared" ref="D123:Q123" si="32">D53*53.11/1000</f>
         <v>0</v>
@@ -9099,10 +9127,10 @@
     </row>
     <row r="124" spans="1:35" ht="22.5" customHeight="1">
       <c r="A124" s="44"/>
-      <c r="B124" s="154" t="s">
+      <c r="B124" s="186" t="s">
         <v>99</v>
       </c>
-      <c r="C124" s="154"/>
+      <c r="C124" s="186"/>
       <c r="D124" s="139">
         <f t="shared" ref="D124:Q124" si="33">D54*74.33/1000</f>
         <v>0</v>
@@ -9180,10 +9208,10 @@
     </row>
     <row r="125" spans="1:35" ht="22.5" customHeight="1">
       <c r="A125" s="44"/>
-      <c r="B125" s="154" t="s">
+      <c r="B125" s="186" t="s">
         <v>100</v>
       </c>
-      <c r="C125" s="154"/>
+      <c r="C125" s="186"/>
       <c r="D125" s="139">
         <f t="shared" ref="D125:Q125" si="34">D55*64.25/1000</f>
         <v>0</v>
@@ -9261,10 +9289,10 @@
     </row>
     <row r="126" spans="1:35" ht="22.5" customHeight="1">
       <c r="A126" s="44"/>
-      <c r="B126" s="154" t="s">
+      <c r="B126" s="186" t="s">
         <v>101</v>
       </c>
-      <c r="C126" s="154"/>
+      <c r="C126" s="186"/>
       <c r="D126" s="139">
         <f t="shared" ref="D126:Q126" si="35">D56*114.42/1000</f>
         <v>0</v>
@@ -9342,10 +9370,10 @@
     </row>
     <row r="127" spans="1:35" ht="22.5" customHeight="1">
       <c r="A127" s="44"/>
-      <c r="B127" s="154" t="s">
+      <c r="B127" s="186" t="s">
         <v>102</v>
       </c>
-      <c r="C127" s="154"/>
+      <c r="C127" s="186"/>
       <c r="D127" s="139">
         <f t="shared" ref="D127:Q127" si="36">D57*99.235/1000</f>
         <v>0</v>
@@ -9423,10 +9451,10 @@
     </row>
     <row r="128" spans="1:35" ht="32.25" customHeight="1">
       <c r="A128" s="44"/>
-      <c r="B128" s="154" t="s">
+      <c r="B128" s="186" t="s">
         <v>103</v>
       </c>
-      <c r="C128" s="154"/>
+      <c r="C128" s="186"/>
       <c r="D128" s="139">
         <f t="shared" ref="D128:Q128" si="37">D58*75.35/1000</f>
         <v>0</v>
@@ -9504,10 +9532,10 @@
     </row>
     <row r="129" spans="1:35" ht="22.5" customHeight="1">
       <c r="A129" s="44"/>
-      <c r="B129" s="155" t="s">
+      <c r="B129" s="187" t="s">
         <v>104</v>
       </c>
-      <c r="C129" s="155"/>
+      <c r="C129" s="187"/>
       <c r="D129" s="139">
         <f t="shared" ref="D129:Q129" si="38">D59*95.05/1000</f>
         <v>0</v>
@@ -9585,10 +9613,10 @@
     </row>
     <row r="130" spans="1:35" ht="22.5" customHeight="1">
       <c r="A130" s="44"/>
-      <c r="B130" s="155" t="s">
+      <c r="B130" s="187" t="s">
         <v>105</v>
       </c>
-      <c r="C130" s="155"/>
+      <c r="C130" s="187"/>
       <c r="D130" s="144"/>
       <c r="E130" s="144"/>
       <c r="F130" s="144"/>
@@ -9624,10 +9652,10 @@
     </row>
     <row r="131" spans="1:35" ht="22.5" customHeight="1">
       <c r="A131" s="44"/>
-      <c r="B131" s="155" t="s">
+      <c r="B131" s="187" t="s">
         <v>106</v>
       </c>
-      <c r="C131" s="155"/>
+      <c r="C131" s="187"/>
       <c r="D131" s="144"/>
       <c r="E131" s="144"/>
       <c r="F131" s="144"/>
@@ -9663,10 +9691,10 @@
     </row>
     <row r="132" spans="1:35" ht="22.5" customHeight="1">
       <c r="A132" s="44"/>
-      <c r="B132" s="155" t="s">
+      <c r="B132" s="187" t="s">
         <v>107</v>
       </c>
-      <c r="C132" s="155"/>
+      <c r="C132" s="187"/>
       <c r="D132" s="139">
         <f t="shared" ref="D132:Q132" si="39">D62*70.66/1000</f>
         <v>0</v>
@@ -9744,10 +9772,10 @@
     </row>
     <row r="133" spans="1:35" ht="22.5" customHeight="1">
       <c r="A133" s="44"/>
-      <c r="B133" s="155" t="s">
+      <c r="B133" s="187" t="s">
         <v>108</v>
       </c>
-      <c r="C133" s="155"/>
+      <c r="C133" s="187"/>
       <c r="D133" s="139">
         <f t="shared" ref="D133:Q133" si="40">D63*74.21/1000</f>
         <v>0</v>
@@ -9825,10 +9853,10 @@
     </row>
     <row r="134" spans="1:35" ht="22.5" customHeight="1">
       <c r="A134" s="44"/>
-      <c r="B134" s="155" t="s">
+      <c r="B134" s="187" t="s">
         <v>109</v>
       </c>
-      <c r="C134" s="155"/>
+      <c r="C134" s="187"/>
       <c r="D134" s="144"/>
       <c r="E134" s="144"/>
       <c r="F134" s="144"/>
@@ -9944,10 +9972,10 @@
     </row>
     <row r="136" spans="1:35" ht="22.5" customHeight="1">
       <c r="A136" s="44"/>
-      <c r="B136" s="155" t="s">
+      <c r="B136" s="187" t="s">
         <v>111</v>
       </c>
-      <c r="C136" s="155"/>
+      <c r="C136" s="187"/>
       <c r="D136" s="139">
         <f t="shared" ref="D136:Q136" si="42">D66*53.11/1000</f>
         <v>0</v>
@@ -28686,107 +28714,6 @@
     </row>
   </sheetData>
   <mergeCells count="118">
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="B7:Q7"/>
-    <mergeCell ref="B8:Q8"/>
-    <mergeCell ref="D10:M10"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:Q22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="T29:U29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="T30:U30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="T33:U33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B36:Q36"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B41:Q41"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="S44:T44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="S50:T50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="S53:T53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B72:Q72"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="S75:T75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="S77:T77"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B85:Q85"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B93:Q93"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B115:Q115"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
     <mergeCell ref="B128:C128"/>
     <mergeCell ref="B129:C129"/>
     <mergeCell ref="B130:C130"/>
@@ -28804,8 +28731,109 @@
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="B126:C126"/>
     <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B115:Q115"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B93:Q93"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="S77:T77"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B85:Q85"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B72:Q72"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="S75:T75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="S50:T50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="S53:T53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="S44:T44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="S45:T45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="T33:U33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B36:Q36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B41:Q41"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="T29:U29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="T30:U30"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:Q22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B5:Q5"/>
+    <mergeCell ref="B6:Q6"/>
+    <mergeCell ref="B7:Q7"/>
+    <mergeCell ref="B8:Q8"/>
+    <mergeCell ref="D10:M10"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="J13:M13"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation showInputMessage="1" sqref="B15:B21 C21:H21 C15:H18" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -28902,21 +28930,21 @@
       <c r="T3" s="74"/>
     </row>
     <row r="4" spans="1:20" ht="77" customHeight="1">
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="189" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="191"/>
-      <c r="D4" s="191"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="191"/>
-      <c r="G4" s="191"/>
-      <c r="H4" s="191"/>
-      <c r="I4" s="191"/>
-      <c r="J4" s="191"/>
-      <c r="K4" s="191"/>
-      <c r="L4" s="191"/>
-      <c r="M4" s="191"/>
-      <c r="N4" s="192"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
+      <c r="I4" s="190"/>
+      <c r="J4" s="190"/>
+      <c r="K4" s="190"/>
+      <c r="L4" s="190"/>
+      <c r="M4" s="190"/>
+      <c r="N4" s="191"/>
       <c r="O4" s="75"/>
       <c r="Q4" s="75"/>
       <c r="R4" s="75"/>
@@ -28932,20 +28960,20 @@
       <c r="B6" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="193" t="s">
+      <c r="C6" s="192" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="193"/>
-      <c r="J6" s="193"/>
-      <c r="K6" s="193"/>
-      <c r="L6" s="193"/>
-      <c r="M6" s="193"/>
-      <c r="N6" s="193"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="192"/>
+      <c r="K6" s="192"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="192"/>
+      <c r="N6" s="192"/>
       <c r="O6" s="78"/>
       <c r="P6" s="78"/>
       <c r="Q6" s="78"/>
@@ -28954,18 +28982,18 @@
     </row>
     <row r="7" spans="1:20" ht="68.75" customHeight="1">
       <c r="B7" s="79"/>
-      <c r="C7" s="189"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="189"/>
-      <c r="F7" s="189"/>
-      <c r="G7" s="189"/>
-      <c r="H7" s="189"/>
-      <c r="I7" s="189"/>
-      <c r="J7" s="189"/>
-      <c r="K7" s="189"/>
-      <c r="L7" s="189"/>
-      <c r="M7" s="189"/>
-      <c r="N7" s="189"/>
+      <c r="C7" s="193"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="193"/>
+      <c r="J7" s="193"/>
+      <c r="K7" s="193"/>
+      <c r="L7" s="193"/>
+      <c r="M7" s="193"/>
+      <c r="N7" s="193"/>
       <c r="O7" s="80"/>
       <c r="P7" s="80"/>
       <c r="Q7" s="80"/>
@@ -28975,18 +29003,18 @@
     </row>
     <row r="8" spans="1:20" ht="51" customHeight="1">
       <c r="B8" s="79"/>
-      <c r="C8" s="189"/>
-      <c r="D8" s="189"/>
-      <c r="E8" s="189"/>
-      <c r="F8" s="189"/>
-      <c r="G8" s="189"/>
-      <c r="H8" s="189"/>
-      <c r="I8" s="189"/>
-      <c r="J8" s="189"/>
-      <c r="K8" s="189"/>
-      <c r="L8" s="189"/>
-      <c r="M8" s="189"/>
-      <c r="N8" s="189"/>
+      <c r="C8" s="193"/>
+      <c r="D8" s="193"/>
+      <c r="E8" s="193"/>
+      <c r="F8" s="193"/>
+      <c r="G8" s="193"/>
+      <c r="H8" s="193"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="193"/>
+      <c r="K8" s="193"/>
+      <c r="L8" s="193"/>
+      <c r="M8" s="193"/>
+      <c r="N8" s="193"/>
       <c r="O8" s="80"/>
       <c r="P8" s="80"/>
       <c r="Q8" s="80"/>
@@ -28996,18 +29024,18 @@
     </row>
     <row r="9" spans="1:20" ht="51" customHeight="1">
       <c r="B9" s="79"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
-      <c r="F9" s="189"/>
-      <c r="G9" s="189"/>
-      <c r="H9" s="189"/>
-      <c r="I9" s="189"/>
-      <c r="J9" s="189"/>
-      <c r="K9" s="189"/>
-      <c r="L9" s="189"/>
-      <c r="M9" s="189"/>
-      <c r="N9" s="189"/>
+      <c r="C9" s="193"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="193"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="193"/>
+      <c r="L9" s="193"/>
+      <c r="M9" s="193"/>
+      <c r="N9" s="193"/>
       <c r="O9" s="80"/>
       <c r="P9" s="80"/>
       <c r="Q9" s="80"/>
@@ -29017,18 +29045,18 @@
     </row>
     <row r="10" spans="1:20" ht="51" customHeight="1">
       <c r="B10" s="79"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
-      <c r="F10" s="189"/>
-      <c r="G10" s="189"/>
-      <c r="H10" s="189"/>
-      <c r="I10" s="189"/>
-      <c r="J10" s="189"/>
-      <c r="K10" s="189"/>
-      <c r="L10" s="189"/>
-      <c r="M10" s="189"/>
-      <c r="N10" s="189"/>
+      <c r="C10" s="193"/>
+      <c r="D10" s="193"/>
+      <c r="E10" s="193"/>
+      <c r="F10" s="193"/>
+      <c r="G10" s="193"/>
+      <c r="H10" s="193"/>
+      <c r="I10" s="193"/>
+      <c r="J10" s="193"/>
+      <c r="K10" s="193"/>
+      <c r="L10" s="193"/>
+      <c r="M10" s="193"/>
+      <c r="N10" s="193"/>
       <c r="O10" s="80"/>
       <c r="P10" s="80"/>
       <c r="Q10" s="80"/>
@@ -29038,18 +29066,18 @@
     </row>
     <row r="11" spans="1:20" ht="51" customHeight="1">
       <c r="B11" s="79"/>
-      <c r="C11" s="189"/>
-      <c r="D11" s="189"/>
-      <c r="E11" s="189"/>
-      <c r="F11" s="189"/>
-      <c r="G11" s="189"/>
-      <c r="H11" s="189"/>
-      <c r="I11" s="189"/>
-      <c r="J11" s="189"/>
-      <c r="K11" s="189"/>
-      <c r="L11" s="189"/>
-      <c r="M11" s="189"/>
-      <c r="N11" s="189"/>
+      <c r="C11" s="193"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="193"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="193"/>
+      <c r="H11" s="193"/>
+      <c r="I11" s="193"/>
+      <c r="J11" s="193"/>
+      <c r="K11" s="193"/>
+      <c r="L11" s="193"/>
+      <c r="M11" s="193"/>
+      <c r="N11" s="193"/>
       <c r="O11" s="80"/>
       <c r="P11" s="80"/>
       <c r="Q11" s="80"/>
@@ -29059,18 +29087,18 @@
     </row>
     <row r="12" spans="1:20" ht="51" customHeight="1">
       <c r="B12" s="79"/>
-      <c r="C12" s="189"/>
-      <c r="D12" s="189"/>
-      <c r="E12" s="189"/>
-      <c r="F12" s="189"/>
-      <c r="G12" s="189"/>
-      <c r="H12" s="189"/>
-      <c r="I12" s="189"/>
-      <c r="J12" s="189"/>
-      <c r="K12" s="189"/>
-      <c r="L12" s="189"/>
-      <c r="M12" s="189"/>
-      <c r="N12" s="189"/>
+      <c r="C12" s="193"/>
+      <c r="D12" s="193"/>
+      <c r="E12" s="193"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="193"/>
+      <c r="H12" s="193"/>
+      <c r="I12" s="193"/>
+      <c r="J12" s="193"/>
+      <c r="K12" s="193"/>
+      <c r="L12" s="193"/>
+      <c r="M12" s="193"/>
+      <c r="N12" s="193"/>
       <c r="O12" s="80"/>
       <c r="P12" s="80"/>
       <c r="Q12" s="80"/>
@@ -29080,18 +29108,18 @@
     </row>
     <row r="13" spans="1:20" ht="51" customHeight="1">
       <c r="B13" s="79"/>
-      <c r="C13" s="189"/>
-      <c r="D13" s="189"/>
-      <c r="E13" s="189"/>
-      <c r="F13" s="189"/>
-      <c r="G13" s="189"/>
-      <c r="H13" s="189"/>
-      <c r="I13" s="189"/>
-      <c r="J13" s="189"/>
-      <c r="K13" s="189"/>
-      <c r="L13" s="189"/>
-      <c r="M13" s="189"/>
-      <c r="N13" s="189"/>
+      <c r="C13" s="193"/>
+      <c r="D13" s="193"/>
+      <c r="E13" s="193"/>
+      <c r="F13" s="193"/>
+      <c r="G13" s="193"/>
+      <c r="H13" s="193"/>
+      <c r="I13" s="193"/>
+      <c r="J13" s="193"/>
+      <c r="K13" s="193"/>
+      <c r="L13" s="193"/>
+      <c r="M13" s="193"/>
+      <c r="N13" s="193"/>
       <c r="O13" s="80"/>
       <c r="P13" s="80"/>
       <c r="Q13" s="80"/>
@@ -29101,18 +29129,18 @@
     </row>
     <row r="14" spans="1:20" ht="51" customHeight="1">
       <c r="B14" s="79"/>
-      <c r="C14" s="189"/>
-      <c r="D14" s="189"/>
-      <c r="E14" s="189"/>
-      <c r="F14" s="189"/>
-      <c r="G14" s="189"/>
-      <c r="H14" s="189"/>
-      <c r="I14" s="189"/>
-      <c r="J14" s="189"/>
-      <c r="K14" s="189"/>
-      <c r="L14" s="189"/>
-      <c r="M14" s="189"/>
-      <c r="N14" s="189"/>
+      <c r="C14" s="193"/>
+      <c r="D14" s="193"/>
+      <c r="E14" s="193"/>
+      <c r="F14" s="193"/>
+      <c r="G14" s="193"/>
+      <c r="H14" s="193"/>
+      <c r="I14" s="193"/>
+      <c r="J14" s="193"/>
+      <c r="K14" s="193"/>
+      <c r="L14" s="193"/>
+      <c r="M14" s="193"/>
+      <c r="N14" s="193"/>
       <c r="O14" s="80"/>
       <c r="P14" s="80"/>
       <c r="Q14" s="80"/>
@@ -29122,18 +29150,18 @@
     </row>
     <row r="15" spans="1:20" ht="51" customHeight="1">
       <c r="B15" s="79"/>
-      <c r="C15" s="189"/>
-      <c r="D15" s="189"/>
-      <c r="E15" s="189"/>
-      <c r="F15" s="189"/>
-      <c r="G15" s="189"/>
-      <c r="H15" s="189"/>
-      <c r="I15" s="189"/>
-      <c r="J15" s="189"/>
-      <c r="K15" s="189"/>
-      <c r="L15" s="189"/>
-      <c r="M15" s="189"/>
-      <c r="N15" s="189"/>
+      <c r="C15" s="193"/>
+      <c r="D15" s="193"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="193"/>
+      <c r="K15" s="193"/>
+      <c r="L15" s="193"/>
+      <c r="M15" s="193"/>
+      <c r="N15" s="193"/>
       <c r="O15" s="80"/>
       <c r="P15" s="80"/>
       <c r="Q15" s="80"/>
@@ -29143,18 +29171,18 @@
     </row>
     <row r="16" spans="1:20" ht="51" customHeight="1">
       <c r="B16" s="79"/>
-      <c r="C16" s="189"/>
-      <c r="D16" s="189"/>
-      <c r="E16" s="189"/>
-      <c r="F16" s="189"/>
-      <c r="G16" s="189"/>
-      <c r="H16" s="189"/>
-      <c r="I16" s="189"/>
-      <c r="J16" s="189"/>
-      <c r="K16" s="189"/>
-      <c r="L16" s="189"/>
-      <c r="M16" s="189"/>
-      <c r="N16" s="189"/>
+      <c r="C16" s="193"/>
+      <c r="D16" s="193"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
+      <c r="K16" s="193"/>
+      <c r="L16" s="193"/>
+      <c r="M16" s="193"/>
+      <c r="N16" s="193"/>
       <c r="O16" s="80"/>
       <c r="P16" s="80"/>
       <c r="Q16" s="80"/>
@@ -29164,18 +29192,18 @@
     </row>
     <row r="17" spans="2:20" ht="51" customHeight="1">
       <c r="B17" s="79"/>
-      <c r="C17" s="189"/>
-      <c r="D17" s="189"/>
-      <c r="E17" s="189"/>
-      <c r="F17" s="189"/>
-      <c r="G17" s="189"/>
-      <c r="H17" s="189"/>
-      <c r="I17" s="189"/>
-      <c r="J17" s="189"/>
-      <c r="K17" s="189"/>
-      <c r="L17" s="189"/>
-      <c r="M17" s="189"/>
-      <c r="N17" s="189"/>
+      <c r="C17" s="193"/>
+      <c r="D17" s="193"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="193"/>
+      <c r="L17" s="193"/>
+      <c r="M17" s="193"/>
+      <c r="N17" s="193"/>
       <c r="O17" s="80"/>
       <c r="P17" s="80"/>
       <c r="Q17" s="80"/>
@@ -29345,11 +29373,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C9:N9"/>
     <mergeCell ref="C15:N15"/>
     <mergeCell ref="C16:N16"/>
     <mergeCell ref="C17:N17"/>
@@ -29358,6 +29381,11 @@
     <mergeCell ref="C12:N12"/>
     <mergeCell ref="C13:N13"/>
     <mergeCell ref="C14:N14"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
+    <mergeCell ref="C9:N9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation showInputMessage="1" sqref="P8:S8" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
@@ -29440,15 +29468,15 @@
       <c r="N3" s="74"/>
     </row>
     <row r="4" spans="1:16" ht="50.75" customHeight="1">
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="189" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="191"/>
-      <c r="D4" s="191"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="191"/>
-      <c r="G4" s="191"/>
-      <c r="H4" s="192"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="191"/>
       <c r="I4" s="75"/>
       <c r="J4" s="75"/>
       <c r="K4" s="75"/>
@@ -29832,21 +29860,21 @@
       <c r="T3" s="74"/>
     </row>
     <row r="4" spans="1:20" ht="39" customHeight="1">
-      <c r="B4" s="190" t="s">
+      <c r="B4" s="189" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="191"/>
-      <c r="D4" s="191"/>
-      <c r="E4" s="191"/>
-      <c r="F4" s="191"/>
-      <c r="G4" s="191"/>
-      <c r="H4" s="191"/>
-      <c r="I4" s="191"/>
-      <c r="J4" s="191"/>
-      <c r="K4" s="191"/>
-      <c r="L4" s="191"/>
-      <c r="M4" s="191"/>
-      <c r="N4" s="192"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
+      <c r="I4" s="190"/>
+      <c r="J4" s="190"/>
+      <c r="K4" s="190"/>
+      <c r="L4" s="190"/>
+      <c r="M4" s="190"/>
+      <c r="N4" s="191"/>
       <c r="O4" s="75"/>
       <c r="P4" s="75"/>
       <c r="Q4" s="75"/>
@@ -29863,20 +29891,20 @@
       <c r="B6" s="77" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="193" t="s">
+      <c r="C6" s="192" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="193"/>
-      <c r="H6" s="193"/>
-      <c r="I6" s="193"/>
-      <c r="J6" s="193"/>
-      <c r="K6" s="193"/>
-      <c r="L6" s="193"/>
-      <c r="M6" s="193"/>
-      <c r="N6" s="193"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="192"/>
+      <c r="K6" s="192"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="192"/>
+      <c r="N6" s="192"/>
       <c r="O6" s="78"/>
       <c r="P6" s="78"/>
       <c r="Q6" s="78"/>
@@ -29885,18 +29913,18 @@
     </row>
     <row r="7" spans="1:20" ht="51" customHeight="1">
       <c r="B7" s="79"/>
-      <c r="C7" s="189"/>
-      <c r="D7" s="189"/>
-      <c r="E7" s="189"/>
-      <c r="F7" s="189"/>
-      <c r="G7" s="189"/>
-      <c r="H7" s="189"/>
-      <c r="I7" s="189"/>
-      <c r="J7" s="189"/>
-      <c r="K7" s="189"/>
-      <c r="L7" s="189"/>
-      <c r="M7" s="189"/>
-      <c r="N7" s="189"/>
+      <c r="C7" s="193"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="193"/>
+      <c r="J7" s="193"/>
+      <c r="K7" s="193"/>
+      <c r="L7" s="193"/>
+      <c r="M7" s="193"/>
+      <c r="N7" s="193"/>
       <c r="O7" s="80"/>
       <c r="P7" s="80"/>
       <c r="Q7" s="80"/>
@@ -29906,18 +29934,18 @@
     </row>
     <row r="8" spans="1:20" ht="51" customHeight="1">
       <c r="B8" s="152"/>
-      <c r="C8" s="189"/>
-      <c r="D8" s="189"/>
-      <c r="E8" s="189"/>
-      <c r="F8" s="189"/>
-      <c r="G8" s="189"/>
-      <c r="H8" s="189"/>
-      <c r="I8" s="189"/>
-      <c r="J8" s="189"/>
-      <c r="K8" s="189"/>
-      <c r="L8" s="189"/>
-      <c r="M8" s="189"/>
-      <c r="N8" s="189"/>
+      <c r="C8" s="193"/>
+      <c r="D8" s="193"/>
+      <c r="E8" s="193"/>
+      <c r="F8" s="193"/>
+      <c r="G8" s="193"/>
+      <c r="H8" s="193"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="193"/>
+      <c r="K8" s="193"/>
+      <c r="L8" s="193"/>
+      <c r="M8" s="193"/>
+      <c r="N8" s="193"/>
       <c r="O8" s="80"/>
       <c r="P8" s="80"/>
       <c r="Q8" s="80"/>
@@ -29927,18 +29955,18 @@
     </row>
     <row r="9" spans="1:20" ht="51" customHeight="1">
       <c r="B9" s="79"/>
-      <c r="C9" s="189"/>
-      <c r="D9" s="189"/>
-      <c r="E9" s="189"/>
-      <c r="F9" s="189"/>
-      <c r="G9" s="189"/>
-      <c r="H9" s="189"/>
-      <c r="I9" s="189"/>
-      <c r="J9" s="189"/>
-      <c r="K9" s="189"/>
-      <c r="L9" s="189"/>
-      <c r="M9" s="189"/>
-      <c r="N9" s="189"/>
+      <c r="C9" s="193"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="193"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="193"/>
+      <c r="L9" s="193"/>
+      <c r="M9" s="193"/>
+      <c r="N9" s="193"/>
       <c r="O9" s="80"/>
       <c r="P9" s="80"/>
       <c r="Q9" s="80"/>
@@ -29948,18 +29976,18 @@
     </row>
     <row r="10" spans="1:20" ht="51" customHeight="1">
       <c r="B10" s="79"/>
-      <c r="C10" s="189"/>
-      <c r="D10" s="189"/>
-      <c r="E10" s="189"/>
-      <c r="F10" s="189"/>
-      <c r="G10" s="189"/>
-      <c r="H10" s="189"/>
-      <c r="I10" s="189"/>
-      <c r="J10" s="189"/>
-      <c r="K10" s="189"/>
-      <c r="L10" s="189"/>
-      <c r="M10" s="189"/>
-      <c r="N10" s="189"/>
+      <c r="C10" s="193"/>
+      <c r="D10" s="193"/>
+      <c r="E10" s="193"/>
+      <c r="F10" s="193"/>
+      <c r="G10" s="193"/>
+      <c r="H10" s="193"/>
+      <c r="I10" s="193"/>
+      <c r="J10" s="193"/>
+      <c r="K10" s="193"/>
+      <c r="L10" s="193"/>
+      <c r="M10" s="193"/>
+      <c r="N10" s="193"/>
       <c r="O10" s="80"/>
       <c r="P10" s="80"/>
       <c r="Q10" s="80"/>
@@ -29969,18 +29997,18 @@
     </row>
     <row r="11" spans="1:20" ht="51" customHeight="1">
       <c r="B11" s="79"/>
-      <c r="C11" s="189"/>
-      <c r="D11" s="189"/>
-      <c r="E11" s="189"/>
-      <c r="F11" s="189"/>
-      <c r="G11" s="189"/>
-      <c r="H11" s="189"/>
-      <c r="I11" s="189"/>
-      <c r="J11" s="189"/>
-      <c r="K11" s="189"/>
-      <c r="L11" s="189"/>
-      <c r="M11" s="189"/>
-      <c r="N11" s="189"/>
+      <c r="C11" s="193"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="193"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="193"/>
+      <c r="H11" s="193"/>
+      <c r="I11" s="193"/>
+      <c r="J11" s="193"/>
+      <c r="K11" s="193"/>
+      <c r="L11" s="193"/>
+      <c r="M11" s="193"/>
+      <c r="N11" s="193"/>
       <c r="O11" s="80"/>
       <c r="P11" s="80"/>
       <c r="Q11" s="80"/>
@@ -29990,18 +30018,18 @@
     </row>
     <row r="12" spans="1:20" ht="51" customHeight="1">
       <c r="B12" s="79"/>
-      <c r="C12" s="189"/>
-      <c r="D12" s="189"/>
-      <c r="E12" s="189"/>
-      <c r="F12" s="189"/>
-      <c r="G12" s="189"/>
-      <c r="H12" s="189"/>
-      <c r="I12" s="189"/>
-      <c r="J12" s="189"/>
-      <c r="K12" s="189"/>
-      <c r="L12" s="189"/>
-      <c r="M12" s="189"/>
-      <c r="N12" s="189"/>
+      <c r="C12" s="193"/>
+      <c r="D12" s="193"/>
+      <c r="E12" s="193"/>
+      <c r="F12" s="193"/>
+      <c r="G12" s="193"/>
+      <c r="H12" s="193"/>
+      <c r="I12" s="193"/>
+      <c r="J12" s="193"/>
+      <c r="K12" s="193"/>
+      <c r="L12" s="193"/>
+      <c r="M12" s="193"/>
+      <c r="N12" s="193"/>
       <c r="O12" s="80"/>
       <c r="P12" s="80"/>
       <c r="Q12" s="80"/>
@@ -30011,18 +30039,18 @@
     </row>
     <row r="13" spans="1:20" ht="51" customHeight="1">
       <c r="B13" s="79"/>
-      <c r="C13" s="189"/>
-      <c r="D13" s="189"/>
-      <c r="E13" s="189"/>
-      <c r="F13" s="189"/>
-      <c r="G13" s="189"/>
-      <c r="H13" s="189"/>
-      <c r="I13" s="189"/>
-      <c r="J13" s="189"/>
-      <c r="K13" s="189"/>
-      <c r="L13" s="189"/>
-      <c r="M13" s="189"/>
-      <c r="N13" s="189"/>
+      <c r="C13" s="193"/>
+      <c r="D13" s="193"/>
+      <c r="E13" s="193"/>
+      <c r="F13" s="193"/>
+      <c r="G13" s="193"/>
+      <c r="H13" s="193"/>
+      <c r="I13" s="193"/>
+      <c r="J13" s="193"/>
+      <c r="K13" s="193"/>
+      <c r="L13" s="193"/>
+      <c r="M13" s="193"/>
+      <c r="N13" s="193"/>
       <c r="O13" s="80"/>
       <c r="P13" s="80"/>
       <c r="Q13" s="80"/>
@@ -30032,18 +30060,18 @@
     </row>
     <row r="14" spans="1:20" ht="51" customHeight="1">
       <c r="B14" s="79"/>
-      <c r="C14" s="189"/>
-      <c r="D14" s="189"/>
-      <c r="E14" s="189"/>
-      <c r="F14" s="189"/>
-      <c r="G14" s="189"/>
-      <c r="H14" s="189"/>
-      <c r="I14" s="189"/>
-      <c r="J14" s="189"/>
-      <c r="K14" s="189"/>
-      <c r="L14" s="189"/>
-      <c r="M14" s="189"/>
-      <c r="N14" s="189"/>
+      <c r="C14" s="193"/>
+      <c r="D14" s="193"/>
+      <c r="E14" s="193"/>
+      <c r="F14" s="193"/>
+      <c r="G14" s="193"/>
+      <c r="H14" s="193"/>
+      <c r="I14" s="193"/>
+      <c r="J14" s="193"/>
+      <c r="K14" s="193"/>
+      <c r="L14" s="193"/>
+      <c r="M14" s="193"/>
+      <c r="N14" s="193"/>
       <c r="O14" s="80"/>
       <c r="P14" s="80"/>
       <c r="Q14" s="80"/>
@@ -30053,18 +30081,18 @@
     </row>
     <row r="15" spans="1:20" ht="51" customHeight="1">
       <c r="B15" s="79"/>
-      <c r="C15" s="189"/>
-      <c r="D15" s="189"/>
-      <c r="E15" s="189"/>
-      <c r="F15" s="189"/>
-      <c r="G15" s="189"/>
-      <c r="H15" s="189"/>
-      <c r="I15" s="189"/>
-      <c r="J15" s="189"/>
-      <c r="K15" s="189"/>
-      <c r="L15" s="189"/>
-      <c r="M15" s="189"/>
-      <c r="N15" s="189"/>
+      <c r="C15" s="193"/>
+      <c r="D15" s="193"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="193"/>
+      <c r="K15" s="193"/>
+      <c r="L15" s="193"/>
+      <c r="M15" s="193"/>
+      <c r="N15" s="193"/>
       <c r="O15" s="80"/>
       <c r="P15" s="80"/>
       <c r="Q15" s="80"/>
@@ -30074,18 +30102,18 @@
     </row>
     <row r="16" spans="1:20" ht="51" customHeight="1">
       <c r="B16" s="79"/>
-      <c r="C16" s="189"/>
-      <c r="D16" s="189"/>
-      <c r="E16" s="189"/>
-      <c r="F16" s="189"/>
-      <c r="G16" s="189"/>
-      <c r="H16" s="189"/>
-      <c r="I16" s="189"/>
-      <c r="J16" s="189"/>
-      <c r="K16" s="189"/>
-      <c r="L16" s="189"/>
-      <c r="M16" s="189"/>
-      <c r="N16" s="189"/>
+      <c r="C16" s="193"/>
+      <c r="D16" s="193"/>
+      <c r="E16" s="193"/>
+      <c r="F16" s="193"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="193"/>
+      <c r="K16" s="193"/>
+      <c r="L16" s="193"/>
+      <c r="M16" s="193"/>
+      <c r="N16" s="193"/>
       <c r="O16" s="80"/>
       <c r="P16" s="80"/>
       <c r="Q16" s="80"/>
@@ -30095,18 +30123,18 @@
     </row>
     <row r="17" spans="2:20" ht="51" customHeight="1">
       <c r="B17" s="79"/>
-      <c r="C17" s="189"/>
-      <c r="D17" s="189"/>
-      <c r="E17" s="189"/>
-      <c r="F17" s="189"/>
-      <c r="G17" s="189"/>
-      <c r="H17" s="189"/>
-      <c r="I17" s="189"/>
-      <c r="J17" s="189"/>
-      <c r="K17" s="189"/>
-      <c r="L17" s="189"/>
-      <c r="M17" s="189"/>
-      <c r="N17" s="189"/>
+      <c r="C17" s="193"/>
+      <c r="D17" s="193"/>
+      <c r="E17" s="193"/>
+      <c r="F17" s="193"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="193"/>
+      <c r="I17" s="193"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="193"/>
+      <c r="L17" s="193"/>
+      <c r="M17" s="193"/>
+      <c r="N17" s="193"/>
       <c r="O17" s="80"/>
       <c r="P17" s="80"/>
       <c r="Q17" s="80"/>
@@ -30276,11 +30304,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B3:N3"/>
-    <mergeCell ref="B4:N4"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
     <mergeCell ref="C14:N14"/>
     <mergeCell ref="C15:N15"/>
     <mergeCell ref="C16:N16"/>
@@ -30290,6 +30313,11 @@
     <mergeCell ref="C11:N11"/>
     <mergeCell ref="C12:N12"/>
     <mergeCell ref="C13:N13"/>
+    <mergeCell ref="B3:N3"/>
+    <mergeCell ref="B4:N4"/>
+    <mergeCell ref="C6:N6"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C8:N8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation showInputMessage="1" sqref="P8:S8" xr:uid="{00000000-0002-0000-0400-000000000000}"/>

</xml_diff>